<commit_message>
Add Tiramisu's manifest data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="character" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6517" uniqueCount="3273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6519" uniqueCount="3273">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -9853,14 +9853,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="168" formatCode="yyyy&quot;년 &quot;m&quot;월 &quot;d\일"/>
     <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="170" formatCode="yyyy&quot;년 &quot;m&quot;월 &quot;d\일"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -10013,103 +10012,103 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10440,10 +10439,10 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="R156" activeCellId="0" sqref="R156"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="P156" activeCellId="0" sqref="P156:Q156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16704,18 +16703,18 @@
       <c r="F142" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G142" s="6" t="b">
+      <c r="G142" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I142" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J142" s="6" t="b">
+      <c r="I142" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J142" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16742,18 +16741,18 @@
       <c r="F143" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G143" s="6" t="b">
+      <c r="G143" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I143" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J143" s="6" t="b">
+      <c r="I143" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J143" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16786,18 +16785,18 @@
       <c r="F144" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G144" s="6" t="b">
+      <c r="G144" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I144" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J144" s="6" t="b">
+      <c r="I144" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J144" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16824,18 +16823,18 @@
       <c r="F145" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G145" s="6" t="b">
+      <c r="G145" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I145" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J145" s="6" t="b">
+      <c r="I145" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J145" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16868,18 +16867,18 @@
       <c r="F146" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G146" s="6" t="b">
+      <c r="G146" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I146" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J146" s="6" t="b">
+      <c r="I146" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J146" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16906,18 +16905,18 @@
       <c r="F147" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G147" s="6" t="b">
+      <c r="G147" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I147" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J147" s="6" t="b">
+      <c r="I147" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J147" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16959,18 +16958,18 @@
       <c r="F148" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G148" s="6" t="b">
+      <c r="G148" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I148" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J148" s="6" t="b">
+      <c r="I148" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J148" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17009,18 +17008,18 @@
       <c r="F149" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G149" s="6" t="b">
+      <c r="G149" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I149" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J149" s="6" t="b">
+      <c r="I149" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J149" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17047,18 +17046,18 @@
       <c r="F150" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G150" s="6" t="b">
+      <c r="G150" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I150" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J150" s="6" t="b">
+      <c r="I150" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J150" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17100,18 +17099,18 @@
       <c r="F151" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G151" s="6" t="b">
+      <c r="G151" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I151" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J151" s="6" t="b">
+      <c r="I151" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J151" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17144,18 +17143,18 @@
       <c r="F152" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G152" s="6" t="b">
+      <c r="G152" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I152" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J152" s="6" t="b">
+      <c r="I152" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J152" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17182,18 +17181,18 @@
       <c r="F153" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G153" s="6" t="b">
+      <c r="G153" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I153" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J153" s="6" t="b">
+      <c r="I153" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J153" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17235,18 +17234,18 @@
       <c r="F154" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G154" s="6" t="b">
+      <c r="G154" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I154" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J154" s="6" t="b">
+      <c r="I154" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J154" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17279,18 +17278,18 @@
       <c r="F155" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G155" s="6" t="b">
+      <c r="G155" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H155" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I155" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J155" s="6" t="b">
+      <c r="I155" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J155" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17317,18 +17316,18 @@
       <c r="F156" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G156" s="6" t="b">
+      <c r="G156" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I156" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J156" s="6" t="b">
+      <c r="I156" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J156" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17343,6 +17342,12 @@
       </c>
       <c r="N156" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="P156" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q156" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="R156" s="7" t="b">
         <f aca="false">TRUE()</f>
@@ -17368,18 +17373,18 @@
       <c r="F157" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G157" s="6" t="b">
+      <c r="G157" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I157" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J157" s="6" t="b">
+      <c r="I157" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J157" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17412,18 +17417,18 @@
       <c r="F158" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G158" s="6" t="b">
+      <c r="G158" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I158" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J158" s="6" t="b">
+      <c r="I158" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J158" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17450,18 +17455,18 @@
       <c r="F159" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G159" s="6" t="b">
+      <c r="G159" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I159" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J159" s="6" t="b">
+      <c r="I159" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J159" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17497,18 +17502,18 @@
       <c r="F160" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G160" s="6" t="b">
+      <c r="G160" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I160" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J160" s="6" t="b">
+      <c r="I160" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J160" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17541,18 +17546,18 @@
       <c r="F161" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G161" s="6" t="b">
+      <c r="G161" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I161" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J161" s="6" t="b">
+      <c r="I161" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J161" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17579,18 +17584,18 @@
       <c r="F162" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G162" s="6" t="b">
+      <c r="G162" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I162" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J162" s="6" t="b">
+      <c r="I162" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J162" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17626,18 +17631,18 @@
       <c r="F163" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G163" s="6" t="b">
+      <c r="G163" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H163" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I163" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J163" s="6" t="b">
+      <c r="I163" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J163" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17664,18 +17669,18 @@
       <c r="F164" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G164" s="6" t="b">
+      <c r="G164" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I164" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J164" s="6" t="b">
+      <c r="I164" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J164" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17711,18 +17716,18 @@
       <c r="F165" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G165" s="6" t="b">
+      <c r="G165" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I165" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J165" s="6" t="b">
+      <c r="I165" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J165" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17749,18 +17754,18 @@
       <c r="F166" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G166" s="6" t="b">
+      <c r="G166" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I166" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J166" s="6" t="b">
+      <c r="I166" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J166" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17796,18 +17801,18 @@
       <c r="F167" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G167" s="6" t="b">
+      <c r="G167" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I167" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J167" s="6" t="b">
+      <c r="I167" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J167" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17840,18 +17845,18 @@
       <c r="F168" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G168" s="6" t="b">
+      <c r="G168" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I168" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J168" s="6" t="b">
+      <c r="I168" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J168" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17878,18 +17883,18 @@
       <c r="F169" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G169" s="6" t="b">
+      <c r="G169" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H169" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I169" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J169" s="6" t="b">
+      <c r="I169" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J169" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17931,18 +17936,18 @@
       <c r="F170" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G170" s="6" t="b">
+      <c r="G170" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H170" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I170" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J170" s="6" t="b">
+      <c r="I170" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J170" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17981,18 +17986,18 @@
       <c r="F171" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G171" s="6" t="b">
+      <c r="G171" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I171" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J171" s="6" t="b">
+      <c r="I171" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J171" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18019,18 +18024,18 @@
       <c r="F172" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G172" s="6" t="b">
+      <c r="G172" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H172" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I172" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J172" s="6" t="b">
+      <c r="I172" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J172" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18072,18 +18077,18 @@
       <c r="F173" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G173" s="6" t="b">
+      <c r="G173" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H173" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I173" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J173" s="6" t="b">
+      <c r="I173" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J173" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18116,18 +18121,18 @@
       <c r="F174" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="G174" s="6" t="b">
+      <c r="G174" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H174" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I174" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J174" s="6" t="b">
+      <c r="I174" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J174" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26180,7 +26185,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="P156:Q156 H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26590,7 +26595,7 @@
   <dimension ref="A1:G270"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A252" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D271" activeCellId="0" sqref="D271"/>
+      <selection pane="topLeft" activeCell="D271" activeCellId="1" sqref="P156:Q156 D271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30319,7 +30324,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="1" sqref="P156:Q156 A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30696,10 +30701,10 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A604" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C624" activeCellId="0" sqref="C624"/>
+      <selection pane="bottomLeft" activeCell="C624" activeCellId="1" sqref="P156:Q156 C624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add Helena's Stellar Awakening
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="character" sheetId="1" state="visible" r:id="rId3"/>
@@ -10585,10 +10585,10 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N366" activeCellId="0" sqref="N366"/>
+      <selection pane="bottomLeft" activeCell="A253" activeCellId="0" sqref="A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19985,18 +19985,18 @@
       <c r="F213" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G213" s="6" t="b">
+      <c r="G213" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H213" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I213" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J213" s="6" t="b">
+      <c r="I213" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J213" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20029,18 +20029,18 @@
       <c r="F214" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G214" s="6" t="b">
+      <c r="G214" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H214" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I214" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J214" s="6" t="b">
+      <c r="I214" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J214" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20067,18 +20067,18 @@
       <c r="F215" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G215" s="6" t="b">
+      <c r="G215" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I215" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J215" s="6" t="b">
+      <c r="I215" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J215" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20120,18 +20120,18 @@
       <c r="F216" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G216" s="6" t="b">
+      <c r="G216" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H216" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I216" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J216" s="6" t="b">
+      <c r="I216" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J216" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20170,18 +20170,18 @@
       <c r="F217" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="G217" s="6" t="b">
+      <c r="G217" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H217" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I217" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J217" s="6" t="b">
+      <c r="I217" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J217" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20214,18 +20214,18 @@
       <c r="F218" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G218" s="6" t="b">
+      <c r="G218" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I218" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J218" s="6" t="b">
+      <c r="I218" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J218" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20252,18 +20252,18 @@
       <c r="F219" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G219" s="6" t="b">
+      <c r="G219" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H219" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I219" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J219" s="6" t="b">
+      <c r="I219" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J219" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20305,18 +20305,18 @@
       <c r="F220" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G220" s="6" t="b">
+      <c r="G220" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H220" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I220" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J220" s="6" t="b">
+      <c r="I220" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J220" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20343,18 +20343,18 @@
       <c r="F221" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G221" s="6" t="b">
+      <c r="G221" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H221" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I221" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J221" s="6" t="b">
+      <c r="I221" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J221" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20390,18 +20390,18 @@
       <c r="F222" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G222" s="6" t="b">
+      <c r="G222" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H222" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I222" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J222" s="6" t="b">
+      <c r="I222" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J222" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20434,18 +20434,18 @@
       <c r="F223" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G223" s="6" t="b">
+      <c r="G223" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H223" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I223" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J223" s="6" t="b">
+      <c r="I223" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J223" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20472,18 +20472,18 @@
       <c r="F224" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G224" s="6" t="b">
+      <c r="G224" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H224" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I224" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J224" s="6" t="b">
+      <c r="I224" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J224" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20519,18 +20519,18 @@
       <c r="F225" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G225" s="6" t="b">
+      <c r="G225" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H225" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I225" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J225" s="6" t="b">
+      <c r="I225" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J225" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20557,18 +20557,18 @@
       <c r="F226" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G226" s="6" t="b">
+      <c r="G226" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H226" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I226" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J226" s="6" t="b">
+      <c r="I226" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J226" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20604,18 +20604,18 @@
       <c r="F227" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G227" s="6" t="b">
+      <c r="G227" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H227" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I227" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J227" s="6" t="b">
+      <c r="I227" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J227" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20642,18 +20642,18 @@
       <c r="F228" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="G228" s="6" t="b">
+      <c r="G228" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H228" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I228" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J228" s="6" t="b">
+      <c r="I228" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J228" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20677,18 +20677,18 @@
       <c r="F229" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G229" s="6" t="b">
+      <c r="G229" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H229" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I229" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J229" s="6" t="b">
+      <c r="I229" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J229" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20715,18 +20715,18 @@
       <c r="F230" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G230" s="6" t="b">
+      <c r="G230" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H230" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I230" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J230" s="6" t="b">
+      <c r="I230" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J230" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20759,18 +20759,18 @@
       <c r="F231" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G231" s="6" t="b">
+      <c r="G231" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H231" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I231" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J231" s="6" t="b">
+      <c r="I231" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J231" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20800,18 +20800,18 @@
       <c r="F232" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G232" s="6" t="b">
+      <c r="G232" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H232" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I232" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J232" s="6" t="b">
+      <c r="I232" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J232" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20841,18 +20841,18 @@
       <c r="F233" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G233" s="6" t="b">
+      <c r="G233" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H233" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I233" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J233" s="6" t="b">
+      <c r="I233" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J233" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20879,18 +20879,18 @@
       <c r="F234" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G234" s="6" t="b">
+      <c r="G234" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H234" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I234" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J234" s="6" t="b">
+      <c r="I234" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J234" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20923,18 +20923,18 @@
       <c r="F235" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G235" s="6" t="b">
+      <c r="G235" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H235" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I235" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J235" s="6" t="b">
+      <c r="I235" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J235" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20964,18 +20964,18 @@
       <c r="F236" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G236" s="6" t="b">
+      <c r="G236" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H236" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I236" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J236" s="6" t="b">
+      <c r="I236" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J236" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21002,18 +21002,18 @@
       <c r="F237" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G237" s="6" t="b">
+      <c r="G237" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H237" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I237" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J237" s="6" t="b">
+      <c r="I237" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J237" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21046,18 +21046,18 @@
       <c r="F238" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G238" s="6" t="b">
+      <c r="G238" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I238" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J238" s="6" t="b">
+      <c r="I238" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J238" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21084,18 +21084,18 @@
       <c r="F239" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G239" s="6" t="b">
+      <c r="G239" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I239" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J239" s="6" t="b">
+      <c r="I239" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J239" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21128,18 +21128,18 @@
       <c r="F240" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G240" s="6" t="b">
+      <c r="G240" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I240" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J240" s="6" t="b">
+      <c r="I240" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J240" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21166,18 +21166,18 @@
       <c r="F241" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G241" s="6" t="b">
+      <c r="G241" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H241" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I241" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J241" s="6" t="b">
+      <c r="I241" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J241" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21210,18 +21210,18 @@
       <c r="F242" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G242" s="6" t="b">
+      <c r="G242" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I242" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J242" s="6" t="b">
+      <c r="I242" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J242" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21248,18 +21248,18 @@
       <c r="F243" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G243" s="6" t="b">
+      <c r="G243" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H243" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I243" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J243" s="6" t="b">
+      <c r="I243" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J243" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21292,18 +21292,18 @@
       <c r="F244" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G244" s="6" t="b">
+      <c r="G244" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H244" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I244" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J244" s="6" t="b">
+      <c r="I244" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J244" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21330,18 +21330,18 @@
       <c r="F245" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G245" s="6" t="b">
+      <c r="G245" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H245" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I245" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J245" s="6" t="b">
+      <c r="I245" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J245" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21374,18 +21374,18 @@
       <c r="F246" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G246" s="6" t="b">
+      <c r="G246" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H246" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I246" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J246" s="6" t="b">
+      <c r="I246" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J246" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21412,18 +21412,18 @@
       <c r="F247" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G247" s="6" t="b">
+      <c r="G247" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H247" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I247" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J247" s="6" t="b">
+      <c r="I247" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J247" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21456,18 +21456,18 @@
       <c r="F248" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G248" s="6" t="b">
+      <c r="G248" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H248" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I248" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J248" s="6" t="b">
+      <c r="I248" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J248" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21494,18 +21494,18 @@
       <c r="F249" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G249" s="6" t="b">
+      <c r="G249" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H249" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I249" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J249" s="6" t="b">
+      <c r="I249" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J249" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21538,18 +21538,18 @@
       <c r="F250" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G250" s="6" t="b">
+      <c r="G250" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H250" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I250" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J250" s="6" t="b">
+      <c r="I250" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J250" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21576,18 +21576,18 @@
       <c r="F251" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G251" s="6" t="b">
+      <c r="G251" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H251" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I251" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J251" s="6" t="b">
+      <c r="I251" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J251" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21620,18 +21620,18 @@
       <c r="F252" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G252" s="6" t="b">
+      <c r="G252" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I252" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J252" s="6" t="b">
+      <c r="I252" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J252" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21658,18 +21658,18 @@
       <c r="F253" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G253" s="6" t="b">
+      <c r="G253" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I253" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J253" s="6" t="b">
+      <c r="I253" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J253" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21681,6 +21681,10 @@
       </c>
       <c r="N253" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="R253" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21702,18 +21706,18 @@
       <c r="F254" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G254" s="6" t="b">
+      <c r="G254" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H254" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I254" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J254" s="6" t="b">
+      <c r="I254" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J254" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21737,18 +21741,18 @@
       <c r="F255" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G255" s="6" t="b">
+      <c r="G255" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H255" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I255" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J255" s="6" t="b">
+      <c r="I255" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J255" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21775,18 +21779,18 @@
       <c r="F256" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G256" s="6" t="b">
+      <c r="G256" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H256" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I256" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J256" s="6" t="b">
+      <c r="I256" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J256" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21799,7 +21803,7 @@
       <c r="N256" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="R256" s="6" t="b">
+      <c r="R256" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21823,18 +21827,18 @@
       <c r="F257" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G257" s="6" t="b">
+      <c r="G257" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H257" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I257" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J257" s="6" t="b">
+      <c r="I257" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J257" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21861,18 +21865,18 @@
       <c r="F258" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G258" s="6" t="b">
+      <c r="G258" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I258" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J258" s="6" t="b">
+      <c r="I258" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J258" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21905,18 +21909,18 @@
       <c r="F259" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G259" s="6" t="b">
+      <c r="G259" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H259" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I259" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J259" s="6" t="b">
+      <c r="I259" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J259" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21943,18 +21947,18 @@
       <c r="F260" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G260" s="6" t="b">
+      <c r="G260" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H260" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I260" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J260" s="6" t="b">
+      <c r="I260" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J260" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21987,18 +21991,18 @@
       <c r="F261" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G261" s="6" t="b">
+      <c r="G261" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H261" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I261" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J261" s="6" t="b">
+      <c r="I261" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J261" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22032,11 +22036,11 @@
       <c r="H262" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I262" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J262" s="6" t="b">
+      <c r="I262" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J262" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22076,11 +22080,11 @@
       <c r="H263" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I263" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J263" s="6" t="b">
+      <c r="I263" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J263" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22114,11 +22118,11 @@
       <c r="H264" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I264" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J264" s="6" t="b">
+      <c r="I264" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J264" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22158,11 +22162,11 @@
       <c r="H265" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I265" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J265" s="6" t="b">
+      <c r="I265" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J265" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22196,11 +22200,11 @@
       <c r="H266" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I266" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J266" s="6" t="b">
+      <c r="I266" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J266" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22240,11 +22244,11 @@
       <c r="H267" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I267" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J267" s="6" t="b">
+      <c r="I267" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J267" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22284,11 +22288,11 @@
       <c r="H268" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I268" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J268" s="6" t="b">
+      <c r="I268" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J268" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22325,11 +22329,11 @@
       <c r="H269" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I269" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J269" s="6" t="b">
+      <c r="I269" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J269" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22369,11 +22373,11 @@
       <c r="H270" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I270" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J270" s="6" t="b">
+      <c r="I270" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J270" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22386,7 +22390,7 @@
       <c r="N270" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O270" s="6" t="b">
+      <c r="O270" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22417,11 +22421,11 @@
       <c r="H271" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I271" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J271" s="6" t="b">
+      <c r="I271" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J271" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22461,11 +22465,11 @@
       <c r="H272" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I272" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J272" s="6" t="b">
+      <c r="I272" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J272" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22499,11 +22503,11 @@
       <c r="H273" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I273" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J273" s="6" t="b">
+      <c r="I273" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J273" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22546,11 +22550,11 @@
       <c r="H274" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I274" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J274" s="6" t="b">
+      <c r="I274" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J274" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22584,11 +22588,11 @@
       <c r="H275" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I275" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J275" s="6" t="b">
+      <c r="I275" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J275" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22625,11 +22629,11 @@
       <c r="H276" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I276" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J276" s="6" t="b">
+      <c r="I276" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J276" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22669,11 +22673,11 @@
       <c r="H277" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I277" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J277" s="6" t="b">
+      <c r="I277" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J277" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22704,11 +22708,11 @@
       <c r="H278" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I278" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J278" s="6" t="b">
+      <c r="I278" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J278" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22742,11 +22746,11 @@
       <c r="H279" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I279" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J279" s="6" t="b">
+      <c r="I279" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J279" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22786,11 +22790,11 @@
       <c r="H280" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I280" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J280" s="6" t="b">
+      <c r="I280" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J280" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22824,11 +22828,11 @@
       <c r="H281" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I281" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J281" s="6" t="b">
+      <c r="I281" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J281" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22865,11 +22869,11 @@
       <c r="H282" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I282" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J282" s="6" t="b">
+      <c r="I282" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J282" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22909,11 +22913,11 @@
       <c r="H283" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I283" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J283" s="6" t="b">
+      <c r="I283" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J283" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22953,11 +22957,11 @@
       <c r="H284" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I284" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J284" s="6" t="b">
+      <c r="I284" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J284" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22997,11 +23001,11 @@
       <c r="H285" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I285" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J285" s="6" t="b">
+      <c r="I285" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J285" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23041,11 +23045,11 @@
       <c r="H286" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I286" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J286" s="6" t="b">
+      <c r="I286" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J286" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23079,11 +23083,11 @@
       <c r="H287" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I287" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J287" s="6" t="b">
+      <c r="I287" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J287" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23122,11 +23126,11 @@
       <c r="H288" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I288" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J288" s="6" t="b">
+      <c r="I288" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J288" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23139,7 +23143,7 @@
       <c r="N288" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O288" s="6" t="b">
+      <c r="O288" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23170,11 +23174,11 @@
       <c r="H289" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I289" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J289" s="6" t="b">
+      <c r="I289" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J289" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23208,11 +23212,11 @@
       <c r="H290" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I290" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J290" s="6" t="b">
+      <c r="I290" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J290" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23252,11 +23256,11 @@
       <c r="H291" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I291" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J291" s="6" t="b">
+      <c r="I291" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J291" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23293,11 +23297,11 @@
       <c r="H292" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I292" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J292" s="6" t="b">
+      <c r="I292" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J292" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23337,11 +23341,11 @@
       <c r="H293" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I293" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J293" s="6" t="b">
+      <c r="I293" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J293" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23381,11 +23385,11 @@
       <c r="H294" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I294" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J294" s="6" t="b">
+      <c r="I294" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J294" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23425,11 +23429,11 @@
       <c r="H295" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I295" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J295" s="6" t="b">
+      <c r="I295" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J295" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23442,7 +23446,7 @@
       <c r="N295" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O295" s="6" t="b">
+      <c r="O295" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23473,11 +23477,11 @@
       <c r="H296" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I296" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J296" s="6" t="b">
+      <c r="I296" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J296" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23511,11 +23515,11 @@
       <c r="H297" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I297" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J297" s="6" t="b">
+      <c r="I297" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J297" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23555,11 +23559,11 @@
       <c r="H298" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I298" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J298" s="6" t="b">
+      <c r="I298" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J298" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23593,11 +23597,11 @@
       <c r="H299" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I299" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J299" s="6" t="b">
+      <c r="I299" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J299" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23637,11 +23641,11 @@
       <c r="H300" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I300" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J300" s="6" t="b">
+      <c r="I300" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J300" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23675,11 +23679,11 @@
       <c r="H301" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I301" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J301" s="6" t="b">
+      <c r="I301" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J301" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23719,11 +23723,11 @@
       <c r="H302" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I302" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J302" s="6" t="b">
+      <c r="I302" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J302" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23757,11 +23761,11 @@
       <c r="H303" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I303" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J303" s="6" t="b">
+      <c r="I303" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J303" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23801,11 +23805,11 @@
       <c r="H304" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I304" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J304" s="6" t="b">
+      <c r="I304" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J304" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23845,11 +23849,11 @@
       <c r="H305" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I305" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J305" s="6" t="b">
+      <c r="I305" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J305" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23863,7 +23867,7 @@
       <c r="N305" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O305" s="6" t="b">
+      <c r="O305" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23894,11 +23898,11 @@
       <c r="H306" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I306" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J306" s="6" t="b">
+      <c r="I306" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J306" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23938,11 +23942,11 @@
       <c r="H307" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I307" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J307" s="6" t="b">
+      <c r="I307" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J307" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -23976,11 +23980,11 @@
       <c r="H308" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I308" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J308" s="6" t="b">
+      <c r="I308" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J308" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24020,11 +24024,11 @@
       <c r="H309" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I309" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J309" s="6" t="b">
+      <c r="I309" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J309" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24058,11 +24062,11 @@
       <c r="H310" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I310" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J310" s="6" t="b">
+      <c r="I310" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J310" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24102,11 +24106,11 @@
       <c r="H311" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I311" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J311" s="6" t="b">
+      <c r="I311" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J311" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24146,11 +24150,11 @@
       <c r="H312" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I312" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J312" s="6" t="b">
+      <c r="I312" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J312" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24163,7 +24167,7 @@
       <c r="N312" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O312" s="6" t="b">
+      <c r="O312" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24194,11 +24198,11 @@
       <c r="H313" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I313" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J313" s="6" t="b">
+      <c r="I313" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J313" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24238,11 +24242,11 @@
       <c r="H314" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I314" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J314" s="6" t="b">
+      <c r="I314" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J314" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24283,11 +24287,11 @@
       <c r="H315" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I315" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J315" s="6" t="b">
+      <c r="I315" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J315" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24322,11 +24326,11 @@
       <c r="H316" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I316" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J316" s="6" t="b">
+      <c r="I316" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J316" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24367,11 +24371,11 @@
       <c r="H317" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I317" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J317" s="6" t="b">
+      <c r="I317" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J317" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24412,11 +24416,11 @@
       <c r="H318" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I318" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J318" s="6" t="b">
+      <c r="I318" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J318" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24457,11 +24461,11 @@
       <c r="H319" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I319" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J319" s="6" t="b">
+      <c r="I319" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J319" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24474,7 +24478,7 @@
       <c r="N319" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O319" s="6" t="b">
+      <c r="O319" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24506,11 +24510,11 @@
       <c r="H320" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I320" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J320" s="6" t="b">
+      <c r="I320" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J320" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24551,11 +24555,11 @@
       <c r="H321" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I321" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J321" s="6" t="b">
+      <c r="I321" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J321" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24590,11 +24594,11 @@
       <c r="H322" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I322" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J322" s="6" t="b">
+      <c r="I322" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J322" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24635,11 +24639,11 @@
       <c r="H323" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I323" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J323" s="6" t="b">
+      <c r="I323" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J323" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24675,11 +24679,11 @@
       <c r="H324" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I324" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J324" s="6" t="b">
+      <c r="I324" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J324" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24720,11 +24724,11 @@
       <c r="H325" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I325" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J325" s="6" t="b">
+      <c r="I325" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J325" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24765,11 +24769,11 @@
       <c r="H326" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I326" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J326" s="6" t="b">
+      <c r="I326" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J326" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24810,11 +24814,11 @@
       <c r="H327" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I327" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J327" s="6" t="b">
+      <c r="I327" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J327" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24855,11 +24859,11 @@
       <c r="H328" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I328" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J328" s="6" t="b">
+      <c r="I328" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J328" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24872,7 +24876,7 @@
       <c r="N328" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O328" s="6" t="b">
+      <c r="O328" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24904,11 +24908,11 @@
       <c r="H329" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I329" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J329" s="6" t="b">
+      <c r="I329" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J329" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24943,11 +24947,11 @@
       <c r="H330" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I330" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J330" s="6" t="b">
+      <c r="I330" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J330" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24985,11 +24989,11 @@
       <c r="H331" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I331" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J331" s="6" t="b">
+      <c r="I331" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J331" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25028,11 +25032,11 @@
       <c r="H332" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I332" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J332" s="6" t="b">
+      <c r="I332" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J332" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25067,11 +25071,11 @@
       <c r="H333" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I333" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J333" s="6" t="b">
+      <c r="I333" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J333" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25112,11 +25116,11 @@
       <c r="H334" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I334" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J334" s="6" t="b">
+      <c r="I334" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J334" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25130,7 +25134,7 @@
       <c r="N334" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O334" s="6" t="b">
+      <c r="O334" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25162,11 +25166,11 @@
       <c r="H335" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I335" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J335" s="6" t="b">
+      <c r="I335" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J335" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25207,11 +25211,11 @@
       <c r="H336" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I336" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J336" s="6" t="b">
+      <c r="I336" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J336" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25246,11 +25250,11 @@
       <c r="H337" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I337" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J337" s="6" t="b">
+      <c r="I337" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J337" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25288,11 +25292,11 @@
       <c r="H338" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I338" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J338" s="6" t="b">
+      <c r="I338" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J338" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25327,11 +25331,11 @@
       <c r="H339" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I339" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J339" s="6" t="b">
+      <c r="I339" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J339" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25344,7 +25348,7 @@
       <c r="N339" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R339" s="6" t="b">
+      <c r="R339" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25375,11 +25379,11 @@
       <c r="H340" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I340" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J340" s="6" t="b">
+      <c r="I340" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J340" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25414,11 +25418,11 @@
       <c r="H341" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I341" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J341" s="6" t="b">
+      <c r="I341" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J341" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25431,7 +25435,7 @@
       <c r="N341" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="R341" s="6" t="b">
+      <c r="R341" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25462,11 +25466,11 @@
       <c r="H342" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I342" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J342" s="6" t="b">
+      <c r="I342" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J342" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25500,11 +25504,11 @@
       <c r="H343" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I343" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J343" s="6" t="b">
+      <c r="I343" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J343" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25517,7 +25521,7 @@
       <c r="N343" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R343" s="6" t="b">
+      <c r="R343" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25548,11 +25552,11 @@
       <c r="H344" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I344" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J344" s="6" t="b">
+      <c r="I344" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J344" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25586,11 +25590,11 @@
       <c r="H345" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I345" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J345" s="6" t="b">
+      <c r="I345" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J345" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25603,7 +25607,7 @@
       <c r="N345" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R345" s="6" t="b">
+      <c r="R345" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25634,11 +25638,11 @@
       <c r="H346" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I346" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J346" s="6" t="b">
+      <c r="I346" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J346" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25672,11 +25676,11 @@
       <c r="H347" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I347" s="6" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J347" s="6" t="b">
+      <c r="I347" s="1" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J347" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25689,7 +25693,7 @@
       <c r="N347" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R347" s="6" t="b">
+      <c r="R347" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25775,7 +25779,7 @@
       <c r="N349" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R349" s="6" t="b">
+      <c r="R349" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25823,7 +25827,7 @@
       <c r="N350" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R350" s="6" t="b">
+      <c r="R350" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25871,7 +25875,7 @@
       <c r="N351" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R351" s="6" t="b">
+      <c r="R351" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25920,7 +25924,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R352" s="6" t="b">
+      <c r="R352" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26007,7 +26011,7 @@
       <c r="N354" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R354" s="6" t="b">
+      <c r="R354" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26093,7 +26097,7 @@
       <c r="N356" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R356" s="6" t="b">
+      <c r="R356" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26179,7 +26183,7 @@
       <c r="N358" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R358" s="6" t="b">
+      <c r="R358" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26227,7 +26231,7 @@
       <c r="N359" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R359" s="6" t="b">
+      <c r="R359" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26275,7 +26279,7 @@
       <c r="N360" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R360" s="6" t="b">
+      <c r="R360" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26361,7 +26365,7 @@
       <c r="N362" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="R362" s="6" t="b">
+      <c r="R362" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26409,7 +26413,7 @@
       <c r="N363" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R363" s="6" t="b">
+      <c r="R363" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26495,7 +26499,7 @@
       <c r="N365" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R365" s="6" t="b">
+      <c r="R365" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26581,7 +26585,7 @@
       <c r="N367" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R367" s="6" t="b">
+      <c r="R367" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26691,15 +26695,15 @@
       <c r="D2" s="1" t="n">
         <v>289</v>
       </c>
-      <c r="E2" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="b">
+      <c r="E2" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26718,15 +26722,15 @@
       <c r="D3" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="E3" s="3" t="b">
+      <c r="E3" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="b">
+      <c r="F3" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26743,15 +26747,15 @@
         <v>2000000003</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="3" t="b">
+      <c r="E4" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="b">
+      <c r="F4" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26773,15 +26777,15 @@
         <v>2000000004</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="3" t="b">
+      <c r="E5" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="b">
+      <c r="F5" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26803,15 +26807,15 @@
         <v>2000000005</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="3" t="b">
+      <c r="E6" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="b">
+      <c r="F6" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26835,15 +26839,15 @@
       <c r="D7" s="1" t="n">
         <v>309</v>
       </c>
-      <c r="E7" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="b">
+      <c r="E7" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26861,15 +26865,15 @@
         <v>2000000007</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="3" t="b">
+      <c r="E8" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="b">
+      <c r="F8" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26893,15 +26897,15 @@
       <c r="D9" s="1" t="n">
         <v>318</v>
       </c>
-      <c r="E9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="b">
+      <c r="E9" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26921,15 +26925,15 @@
       <c r="D10" s="1" t="n">
         <v>332</v>
       </c>
-      <c r="E10" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="b">
+      <c r="E10" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26946,15 +26950,15 @@
       <c r="C11" s="1" t="n">
         <v>2000000010</v>
       </c>
-      <c r="E11" s="3" t="b">
+      <c r="E11" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="b">
+      <c r="F11" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26978,15 +26982,15 @@
       <c r="D12" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="E12" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3" t="b">
+      <c r="E12" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27004,15 +27008,15 @@
       <c r="D13" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="E13" s="3" t="b">
+      <c r="E13" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F13" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="b">
+      <c r="F13" s="7" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -31208,7 +31212,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A613" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B632" activeCellId="0" sqref="B632"/>

</xml_diff>

<commit_message>
Backup & additional fix
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2271,7 +2271,7 @@
     <t xml:space="preserve">아이스 돌</t>
   </si>
   <si>
-    <t xml:space="preserve">가시나무 저주의 여인 셰이네 </t>
+    <t xml:space="preserve">가시나무 저주의 여인 셰이네</t>
   </si>
   <si>
     <t xml:space="preserve">101070151</t>
@@ -9300,1225 +9300,1225 @@
     <t xml:space="preserve">You don't have this character for now.</t>
   </si>
   <si>
-    <t xml:space="preserve">personality.104</t>
+    <t xml:space="preserve">personality.p000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">무</t>
+  </si>
+  <si>
+    <t xml:space="preserve">無</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">불</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">물</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">바람</t>
+  </si>
+  <si>
+    <t xml:space="preserve">風</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">땅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">그림자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">번개</t>
+  </si>
+  <si>
+    <t xml:space="preserve">雷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">결정</t>
+  </si>
+  <si>
+    <t xml:space="preserve">晶</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">지팡이</t>
+  </si>
+  <si>
+    <t xml:space="preserve">杖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">검</t>
+  </si>
+  <si>
+    <t xml:space="preserve">剣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">도</t>
+  </si>
+  <si>
+    <t xml:space="preserve">刀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">도끼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斧</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">창</t>
+  </si>
+  <si>
+    <t xml:space="preserve">槍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">활</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">권갑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">拳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">망치</t>
+  </si>
+  <si>
+    <t xml:space="preserve">槌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hammer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">왕족</t>
+  </si>
+  <si>
+    <t xml:space="preserve">王族</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">엘프</t>
+  </si>
+  <si>
+    <t xml:space="preserve">エルフ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">정령 대화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">精霊対話</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit Talker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">봉인</t>
+  </si>
+  <si>
+    <t xml:space="preserve">封印</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">과학자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">科学者</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scientist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">로스트 랩</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ロストラボ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost Laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">만능의 지배자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">万能の支配者</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power to Rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">성직자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">聖職者</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서방</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">미술</t>
+  </si>
+  <si>
+    <t xml:space="preserve">美術</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Art</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">애견가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いぬ好き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dog lover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">장비</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">낯가림</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人見知り</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrangement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">독서가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">読書家</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bookworm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">요리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">料理</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">마수</t>
+  </si>
+  <si>
+    <t xml:space="preserve">魔獣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">요괴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">妖し</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">용</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">후드</t>
+  </si>
+  <si>
+    <t xml:space="preserve">フード</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDA스쿨</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDAスクール</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDA School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">북방</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">첩자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">忍び</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">음유시인</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吟遊詩人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">안경</t>
+  </si>
+  <si>
+    <t xml:space="preserve">メガネ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glasses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">콘체르토 아트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">コンチェルトアーツ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concerto Artes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">가면</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仮面</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">천계의 인도</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天の導き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guiding Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">저주</t>
+  </si>
+  <si>
+    <t xml:space="preserve">呪い</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cursed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">낮잠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">お昼寝</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">동물 대화</t>
+  </si>
+  <si>
+    <t xml:space="preserve">動物対話</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal Talker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어인</t>
+  </si>
+  <si>
+    <t xml:space="preserve">魚人</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fishman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">죽마고우</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竹馬の友</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Childhood Friend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">바르오키</t>
+  </si>
+  <si>
+    <t xml:space="preserve">バルオキー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baruoki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">마음의 괴도단</t>
+  </si>
+  <si>
+    <t xml:space="preserve">心の怪盗団</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phantom Thieves of Hearts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">시간의 상흔의 윤무</t>
+  </si>
+  <si>
+    <t xml:space="preserve">時の傷痕の輪舞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scars of the Wheel of Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">영매 체질</t>
+  </si>
+  <si>
+    <t xml:space="preserve">霊媒体質</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit-fused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">단것 애호가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">甘党</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweet tooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">채집</t>
+  </si>
+  <si>
+    <t xml:space="preserve">採集</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">복수</t>
+  </si>
+  <si>
+    <t xml:space="preserve">復讐者</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">생물</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生物</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">상사병</t>
+  </si>
+  <si>
+    <t xml:space="preserve">恋わずらい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovesick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">동방</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">방패</t>
+  </si>
+  <si>
+    <t xml:space="preserve">盾</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shield</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">기억상실</t>
+  </si>
+  <si>
+    <t xml:space="preserve">記憶喪失</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amnesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">명계의 부름</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冥の誘い</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luring Shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">용궁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竜宮</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon Palace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">기계</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マシナリー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machinery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">대식가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大食い</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">테일즈 오브</t>
+  </si>
+  <si>
+    <t xml:space="preserve">テイルズオブ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tales of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">귀가 밝음</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地獄耳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharp Ears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">미글랜스 왕궁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ミグランス王宮</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miglance Palace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">대장간</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鍛冶屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">합성인간</t>
+  </si>
+  <si>
+    <t xml:space="preserve">合成人間</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synth Human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">라이더</t>
+  </si>
+  <si>
+    <t xml:space="preserve">騎乗</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mounted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">무법자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">アウトロー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outlaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">작명가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ニックネーマー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicknamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">프리아레스</t>
+  </si>
+  <si>
+    <t xml:space="preserve">フリアレス</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fleareth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">채굴</t>
+  </si>
+  <si>
+    <t xml:space="preserve">採掘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">드워프</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ドワーフ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dwarf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">장례</t>
+  </si>
+  <si>
+    <t xml:space="preserve">フューネラル</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funeral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">신 몽상 과격단</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新夢想過激団</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Radical Dreamers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">부천수 애호가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">辛党</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spicy Lover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">총</t>
+  </si>
+  <si>
+    <t xml:space="preserve">銃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">타이탄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">タイタン</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">짚단</t>
+  </si>
+  <si>
+    <t xml:space="preserve">巻きワラ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Straw Dummy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">드래곤 킬러</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ドラゴンキラー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragon Killer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">연옥계</t>
+  </si>
+  <si>
+    <t xml:space="preserve">煉獄界</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purgatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">지오</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ジオ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">혐묘가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ねこ嫌い</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat Hater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">미식</t>
+  </si>
+  <si>
+    <t xml:space="preserve">美食</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gourmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">주인공</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主人公</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protagonist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">괭이갈매기 애호가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うみねこ好き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scallywag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMS사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMS社</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">시간 제국</t>
+  </si>
+  <si>
+    <t xml:space="preserve">時間帝国</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chronos Empire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">애묘가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ねこ好き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat lover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">밀리터리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ミリタリー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Military</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">나무꾼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">木こり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woodcutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">연금술사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">錬金術師</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">신 시공 초한 유파</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新時空超限流派</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Time Drift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">보현일도류</t>
+  </si>
+  <si>
+    <t xml:space="preserve">普賢一刀流</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itto-Ryu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">배리몽상단 리더</t>
+  </si>
+  <si>
+    <t xml:space="preserve">背理夢想団リーダー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paradoxical Dreamers Leader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">시간의 황자</t>
+  </si>
+  <si>
+    <t xml:space="preserve">時の皇子</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prince of Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">미래혁명가</t>
+  </si>
+  <si>
+    <t xml:space="preserve">未来革命家</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Future Revolutionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">아르카디아</t>
+  </si>
+  <si>
+    <t xml:space="preserve">アルカディア</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arcadia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">인도의 트래블러</t>
+  </si>
+  <si>
+    <t xml:space="preserve">導きのトラベラー</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traveler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">마검</t>
+  </si>
+  <si>
+    <t xml:space="preserve">魔剣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demon Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personality.p107</t>
   </si>
   <si>
     <t xml:space="preserve">KOF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">무</t>
-  </si>
-  <si>
-    <t xml:space="preserve">無</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">불</t>
-  </si>
-  <si>
-    <t xml:space="preserve">火</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">물</t>
-  </si>
-  <si>
-    <t xml:space="preserve">水</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">바람</t>
-  </si>
-  <si>
-    <t xml:space="preserve">風</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">땅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">地</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">그림자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">陰</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">번개</t>
-  </si>
-  <si>
-    <t xml:space="preserve">雷</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thunder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">결정</t>
-  </si>
-  <si>
-    <t xml:space="preserve">晶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crystal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">지팡이</t>
-  </si>
-  <si>
-    <t xml:space="preserve">杖</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">검</t>
-  </si>
-  <si>
-    <t xml:space="preserve">剣</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">도</t>
-  </si>
-  <si>
-    <t xml:space="preserve">刀</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">도끼</t>
-  </si>
-  <si>
-    <t xml:space="preserve">斧</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">창</t>
-  </si>
-  <si>
-    <t xml:space="preserve">槍</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">활</t>
-  </si>
-  <si>
-    <t xml:space="preserve">弓</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">권갑</t>
-  </si>
-  <si>
-    <t xml:space="preserve">拳</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">망치</t>
-  </si>
-  <si>
-    <t xml:space="preserve">槌</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hammer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">왕족</t>
-  </si>
-  <si>
-    <t xml:space="preserve">王族</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royalty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">엘프</t>
-  </si>
-  <si>
-    <t xml:space="preserve">エルフ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">정령 대화</t>
-  </si>
-  <si>
-    <t xml:space="preserve">精霊対話</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit Talker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">봉인</t>
-  </si>
-  <si>
-    <t xml:space="preserve">封印</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">과학자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">科学者</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scientist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">로스트 랩</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ロストラボ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lost Laboratory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">만능의 지배자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">万能の支配者</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power to Rule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">성직자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">聖職者</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">서방</t>
-  </si>
-  <si>
-    <t xml:space="preserve">西方</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">미술</t>
-  </si>
-  <si>
-    <t xml:space="preserve">美術</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Art</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">애견가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">いぬ好き</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dog lover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">장비</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weapons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">낯가림</t>
-  </si>
-  <si>
-    <t xml:space="preserve">人見知り</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estrangement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">독서가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">読書家</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bookworm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">요리</t>
-  </si>
-  <si>
-    <t xml:space="preserve">料理</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">마수</t>
-  </si>
-  <si>
-    <t xml:space="preserve">魔獣</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">요괴</t>
-  </si>
-  <si>
-    <t xml:space="preserve">妖し</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">용</t>
-  </si>
-  <si>
-    <t xml:space="preserve">竜</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">후드</t>
-  </si>
-  <si>
-    <t xml:space="preserve">フード</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDA스쿨</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDAスクール</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDA School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">북방</t>
-  </si>
-  <si>
-    <t xml:space="preserve">北方</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">첩자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">忍び</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ninja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">음유시인</t>
-  </si>
-  <si>
-    <t xml:space="preserve">吟遊詩人</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">안경</t>
-  </si>
-  <si>
-    <t xml:space="preserve">メガネ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glasses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">콘체르토 아트</t>
-  </si>
-  <si>
-    <t xml:space="preserve">コンチェルトアーツ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concerto Artes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">가면</t>
-  </si>
-  <si>
-    <t xml:space="preserve">仮面</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">천계의 인도</t>
-  </si>
-  <si>
-    <t xml:space="preserve">天の導き</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guiding Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">저주</t>
-  </si>
-  <si>
-    <t xml:space="preserve">呪い</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cursed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">낮잠</t>
-  </si>
-  <si>
-    <t xml:space="preserve">お昼寝</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Napper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">동물 대화</t>
-  </si>
-  <si>
-    <t xml:space="preserve">動物対話</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animal Talker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">어인</t>
-  </si>
-  <si>
-    <t xml:space="preserve">魚人</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fishman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">죽마고우</t>
-  </si>
-  <si>
-    <t xml:space="preserve">竹馬の友</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Childhood Friend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">바르오키</t>
-  </si>
-  <si>
-    <t xml:space="preserve">バルオキー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baruoki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">마음의 괴도단</t>
-  </si>
-  <si>
-    <t xml:space="preserve">心の怪盗団</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phantom Thieves of Hearts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">시간의 상흔의 윤무</t>
-  </si>
-  <si>
-    <t xml:space="preserve">時の傷痕の輪舞</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scars of the Wheel of Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">영매 체질</t>
-  </si>
-  <si>
-    <t xml:space="preserve">霊媒体質</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit-fused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">단것 애호가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">甘党</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweet tooth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">채집</t>
-  </si>
-  <si>
-    <t xml:space="preserve">採集</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">복수</t>
-  </si>
-  <si>
-    <t xml:space="preserve">復讐者</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avenger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">생물</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生物</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">상사병</t>
-  </si>
-  <si>
-    <t xml:space="preserve">恋わずらい</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lovesick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">동방</t>
-  </si>
-  <si>
-    <t xml:space="preserve">東方</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">방패</t>
-  </si>
-  <si>
-    <t xml:space="preserve">盾</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">기억상실</t>
-  </si>
-  <si>
-    <t xml:space="preserve">記憶喪失</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amnesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">명계의 부름</t>
-  </si>
-  <si>
-    <t xml:space="preserve">冥の誘い</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luring Shadow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">용궁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">竜宮</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragon Palace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">기계</t>
-  </si>
-  <si>
-    <t xml:space="preserve">マシナリー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machinery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">대식가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">大食い</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glutton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">테일즈 오브</t>
-  </si>
-  <si>
-    <t xml:space="preserve">テイルズオブ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tales of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">귀가 밝음</t>
-  </si>
-  <si>
-    <t xml:space="preserve">地獄耳</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharp Ears</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">미글랜스 왕궁</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ミグランス王宮</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miglance Palace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">대장간</t>
-  </si>
-  <si>
-    <t xml:space="preserve">鍛冶屋</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">합성인간</t>
-  </si>
-  <si>
-    <t xml:space="preserve">合成人間</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Synth Human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">라이더</t>
-  </si>
-  <si>
-    <t xml:space="preserve">騎乗</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mounted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">무법자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">アウトロー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outlaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">작명가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ニックネーマー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicknamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">프리아레스</t>
-  </si>
-  <si>
-    <t xml:space="preserve">フリアレス</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fleareth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">채굴</t>
-  </si>
-  <si>
-    <t xml:space="preserve">採掘</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">드워프</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ドワーフ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dwarf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">장례</t>
-  </si>
-  <si>
-    <t xml:space="preserve">フューネラル</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funeral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">신 몽상 과격단</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新夢想過激団</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Radical Dreamers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">부천수 애호가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">辛党</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spicy Lover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">총</t>
-  </si>
-  <si>
-    <t xml:space="preserve">銃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">타이탄</t>
-  </si>
-  <si>
-    <t xml:space="preserve">タイタン</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">짚단</t>
-  </si>
-  <si>
-    <t xml:space="preserve">巻きワラ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Straw Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">드래곤 킬러</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ドラゴンキラー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragon Killer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">연옥계</t>
-  </si>
-  <si>
-    <t xml:space="preserve">煉獄界</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purgatory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">지오</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ジオ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">혐묘가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ねこ嫌い</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cat Hater</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">미식</t>
-  </si>
-  <si>
-    <t xml:space="preserve">美食</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gourmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">주인공</t>
-  </si>
-  <si>
-    <t xml:space="preserve">主人公</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Protagonist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">괭이갈매기 애호가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">うみねこ好き</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scallywag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMS사</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMS社</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">시간 제국</t>
-  </si>
-  <si>
-    <t xml:space="preserve">時間帝国</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chronos Empire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">애묘가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ねこ好き</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cat lover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">밀리터리</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ミリタリー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Military</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">나무꾼</t>
-  </si>
-  <si>
-    <t xml:space="preserve">木こり</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woodcutter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">연금술사</t>
-  </si>
-  <si>
-    <t xml:space="preserve">錬金術師</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alchemist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">신 시공 초한 유파</t>
-  </si>
-  <si>
-    <t xml:space="preserve">新時空超限流派</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Time Drift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">보현일도류</t>
-  </si>
-  <si>
-    <t xml:space="preserve">普賢一刀流</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itto-Ryu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">배리몽상단 리더</t>
-  </si>
-  <si>
-    <t xml:space="preserve">背理夢想団リーダー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paradoxical Dreamers Leader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">시간의 황자</t>
-  </si>
-  <si>
-    <t xml:space="preserve">時の皇子</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prince of Time </t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">미래혁명가</t>
-  </si>
-  <si>
-    <t xml:space="preserve">未来革命家</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Future Revolutionary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">아르카디아</t>
-  </si>
-  <si>
-    <t xml:space="preserve">アルカディア</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arcadia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">인도의 트래블러</t>
-  </si>
-  <si>
-    <t xml:space="preserve">導きのトラベラー</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traveler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">personality.p106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">마검</t>
-  </si>
-  <si>
-    <t xml:space="preserve">魔剣</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demon Sword</t>
   </si>
   <si>
     <t xml:space="preserve">staralign.false</t>
@@ -11188,7 +11188,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E394" activeCellId="0" sqref="E394"/>
+      <selection pane="bottomLeft" activeCell="B389" activeCellId="0" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27508,9 +27508,9 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A631" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A643" activeCellId="0" sqref="A643"/>
+      <selection pane="bottomLeft" activeCell="B417" activeCellId="0" sqref="B417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36845,42 +36845,42 @@
         <v>3091</v>
       </c>
       <c r="C549" s="4" t="s">
-        <v>3091</v>
-      </c>
-      <c r="D549" s="4" t="s">
-        <v>3091</v>
-      </c>
-      <c r="E549" s="27" t="n">
-        <v>45528</v>
+        <v>3092</v>
+      </c>
+      <c r="D549" s="3"/>
+      <c r="E549" s="25" t="s">
+        <v>1520</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A550" s="4" t="s">
-        <v>3092</v>
+        <v>3093</v>
       </c>
       <c r="B550" s="4" t="s">
-        <v>3093</v>
+        <v>3094</v>
       </c>
       <c r="C550" s="4" t="s">
-        <v>3094</v>
-      </c>
-      <c r="D550" s="3"/>
+        <v>3095</v>
+      </c>
+      <c r="D550" s="4" t="s">
+        <v>3096</v>
+      </c>
       <c r="E550" s="25" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A551" s="4" t="s">
-        <v>3095</v>
+        <v>3097</v>
       </c>
       <c r="B551" s="4" t="s">
-        <v>3096</v>
+        <v>3098</v>
       </c>
       <c r="C551" s="4" t="s">
-        <v>3097</v>
+        <v>3099</v>
       </c>
       <c r="D551" s="4" t="s">
-        <v>3098</v>
+        <v>3100</v>
       </c>
       <c r="E551" s="25" t="s">
         <v>1520</v>
@@ -36888,16 +36888,16 @@
     </row>
     <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A552" s="4" t="s">
-        <v>3099</v>
+        <v>3101</v>
       </c>
       <c r="B552" s="4" t="s">
-        <v>3100</v>
+        <v>3102</v>
       </c>
       <c r="C552" s="4" t="s">
-        <v>3101</v>
+        <v>3103</v>
       </c>
       <c r="D552" s="4" t="s">
-        <v>3102</v>
+        <v>3104</v>
       </c>
       <c r="E552" s="25" t="s">
         <v>1520</v>
@@ -36905,16 +36905,16 @@
     </row>
     <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A553" s="4" t="s">
-        <v>3103</v>
+        <v>3105</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>3104</v>
+        <v>3106</v>
       </c>
       <c r="C553" s="4" t="s">
-        <v>3105</v>
+        <v>3107</v>
       </c>
       <c r="D553" s="4" t="s">
-        <v>3106</v>
+        <v>3108</v>
       </c>
       <c r="E553" s="25" t="s">
         <v>1520</v>
@@ -36922,16 +36922,16 @@
     </row>
     <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A554" s="4" t="s">
-        <v>3107</v>
+        <v>3109</v>
       </c>
       <c r="B554" s="4" t="s">
-        <v>3108</v>
+        <v>3110</v>
       </c>
       <c r="C554" s="4" t="s">
-        <v>3109</v>
+        <v>3111</v>
       </c>
       <c r="D554" s="4" t="s">
-        <v>3110</v>
+        <v>3112</v>
       </c>
       <c r="E554" s="25" t="s">
         <v>1520</v>
@@ -36939,16 +36939,16 @@
     </row>
     <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A555" s="4" t="s">
-        <v>3111</v>
+        <v>3113</v>
       </c>
       <c r="B555" s="4" t="s">
-        <v>3112</v>
+        <v>3114</v>
       </c>
       <c r="C555" s="4" t="s">
-        <v>3113</v>
+        <v>3115</v>
       </c>
       <c r="D555" s="4" t="s">
-        <v>3114</v>
+        <v>3116</v>
       </c>
       <c r="E555" s="25" t="s">
         <v>1520</v>
@@ -36956,16 +36956,16 @@
     </row>
     <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A556" s="4" t="s">
-        <v>3115</v>
+        <v>3117</v>
       </c>
       <c r="B556" s="4" t="s">
-        <v>3116</v>
+        <v>3118</v>
       </c>
       <c r="C556" s="4" t="s">
-        <v>3117</v>
+        <v>3119</v>
       </c>
       <c r="D556" s="4" t="s">
-        <v>3118</v>
+        <v>3120</v>
       </c>
       <c r="E556" s="25" t="s">
         <v>1520</v>
@@ -36973,16 +36973,16 @@
     </row>
     <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A557" s="4" t="s">
-        <v>3119</v>
+        <v>3121</v>
       </c>
       <c r="B557" s="4" t="s">
-        <v>3120</v>
+        <v>3122</v>
       </c>
       <c r="C557" s="4" t="s">
-        <v>3121</v>
+        <v>3123</v>
       </c>
       <c r="D557" s="4" t="s">
-        <v>3122</v>
+        <v>3124</v>
       </c>
       <c r="E557" s="25" t="s">
         <v>1520</v>
@@ -36990,16 +36990,16 @@
     </row>
     <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A558" s="4" t="s">
-        <v>3123</v>
+        <v>3125</v>
       </c>
       <c r="B558" s="4" t="s">
-        <v>3124</v>
+        <v>3126</v>
       </c>
       <c r="C558" s="4" t="s">
-        <v>3125</v>
+        <v>3127</v>
       </c>
       <c r="D558" s="4" t="s">
-        <v>3126</v>
+        <v>3128</v>
       </c>
       <c r="E558" s="25" t="s">
         <v>1520</v>
@@ -37007,16 +37007,16 @@
     </row>
     <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A559" s="4" t="s">
-        <v>3127</v>
+        <v>3129</v>
       </c>
       <c r="B559" s="4" t="s">
-        <v>3128</v>
+        <v>3130</v>
       </c>
       <c r="C559" s="4" t="s">
-        <v>3129</v>
+        <v>3131</v>
       </c>
       <c r="D559" s="4" t="s">
-        <v>3130</v>
+        <v>3132</v>
       </c>
       <c r="E559" s="25" t="s">
         <v>1520</v>
@@ -37024,16 +37024,16 @@
     </row>
     <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A560" s="4" t="s">
-        <v>3131</v>
+        <v>3133</v>
       </c>
       <c r="B560" s="4" t="s">
-        <v>3132</v>
+        <v>3134</v>
       </c>
       <c r="C560" s="4" t="s">
-        <v>3133</v>
+        <v>3135</v>
       </c>
       <c r="D560" s="4" t="s">
-        <v>3134</v>
+        <v>3136</v>
       </c>
       <c r="E560" s="25" t="s">
         <v>1520</v>
@@ -37041,16 +37041,16 @@
     </row>
     <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A561" s="4" t="s">
-        <v>3135</v>
+        <v>3137</v>
       </c>
       <c r="B561" s="4" t="s">
-        <v>3136</v>
+        <v>3138</v>
       </c>
       <c r="C561" s="4" t="s">
-        <v>3137</v>
+        <v>3139</v>
       </c>
       <c r="D561" s="4" t="s">
-        <v>3138</v>
+        <v>3140</v>
       </c>
       <c r="E561" s="25" t="s">
         <v>1520</v>
@@ -37058,16 +37058,16 @@
     </row>
     <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A562" s="4" t="s">
-        <v>3139</v>
+        <v>3141</v>
       </c>
       <c r="B562" s="4" t="s">
-        <v>3140</v>
+        <v>3142</v>
       </c>
       <c r="C562" s="4" t="s">
-        <v>3141</v>
+        <v>3143</v>
       </c>
       <c r="D562" s="4" t="s">
-        <v>3142</v>
+        <v>3144</v>
       </c>
       <c r="E562" s="25" t="s">
         <v>1520</v>
@@ -37075,16 +37075,16 @@
     </row>
     <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A563" s="4" t="s">
-        <v>3143</v>
+        <v>3145</v>
       </c>
       <c r="B563" s="4" t="s">
-        <v>3144</v>
+        <v>3146</v>
       </c>
       <c r="C563" s="4" t="s">
-        <v>3145</v>
+        <v>3147</v>
       </c>
       <c r="D563" s="4" t="s">
-        <v>3146</v>
+        <v>3148</v>
       </c>
       <c r="E563" s="25" t="s">
         <v>1520</v>
@@ -37092,16 +37092,16 @@
     </row>
     <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A564" s="4" t="s">
-        <v>3147</v>
+        <v>3149</v>
       </c>
       <c r="B564" s="4" t="s">
-        <v>3148</v>
+        <v>3150</v>
       </c>
       <c r="C564" s="4" t="s">
-        <v>3149</v>
+        <v>3151</v>
       </c>
       <c r="D564" s="4" t="s">
-        <v>3150</v>
+        <v>3152</v>
       </c>
       <c r="E564" s="25" t="s">
         <v>1520</v>
@@ -37109,16 +37109,16 @@
     </row>
     <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A565" s="4" t="s">
-        <v>3151</v>
+        <v>3153</v>
       </c>
       <c r="B565" s="4" t="s">
-        <v>3152</v>
+        <v>3154</v>
       </c>
       <c r="C565" s="4" t="s">
-        <v>3153</v>
+        <v>3155</v>
       </c>
       <c r="D565" s="4" t="s">
-        <v>3154</v>
+        <v>3156</v>
       </c>
       <c r="E565" s="25" t="s">
         <v>1520</v>
@@ -37126,16 +37126,16 @@
     </row>
     <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A566" s="4" t="s">
-        <v>3155</v>
+        <v>3157</v>
       </c>
       <c r="B566" s="4" t="s">
-        <v>3156</v>
+        <v>3158</v>
       </c>
       <c r="C566" s="4" t="s">
-        <v>3157</v>
+        <v>3159</v>
       </c>
       <c r="D566" s="4" t="s">
-        <v>3158</v>
+        <v>3160</v>
       </c>
       <c r="E566" s="25" t="s">
         <v>1520</v>
@@ -37143,16 +37143,16 @@
     </row>
     <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A567" s="4" t="s">
-        <v>3159</v>
+        <v>3161</v>
       </c>
       <c r="B567" s="4" t="s">
-        <v>3160</v>
+        <v>3162</v>
       </c>
       <c r="C567" s="4" t="s">
-        <v>3161</v>
+        <v>3163</v>
       </c>
       <c r="D567" s="4" t="s">
-        <v>3162</v>
+        <v>3164</v>
       </c>
       <c r="E567" s="25" t="s">
         <v>1520</v>
@@ -37160,16 +37160,16 @@
     </row>
     <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A568" s="4" t="s">
-        <v>3163</v>
+        <v>3165</v>
       </c>
       <c r="B568" s="4" t="s">
-        <v>3164</v>
+        <v>3166</v>
       </c>
       <c r="C568" s="4" t="s">
-        <v>3165</v>
+        <v>3167</v>
       </c>
       <c r="D568" s="4" t="s">
-        <v>3166</v>
+        <v>3168</v>
       </c>
       <c r="E568" s="25" t="s">
         <v>1520</v>
@@ -37177,16 +37177,16 @@
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A569" s="4" t="s">
-        <v>3167</v>
+        <v>3169</v>
       </c>
       <c r="B569" s="4" t="s">
-        <v>3168</v>
+        <v>3170</v>
       </c>
       <c r="C569" s="4" t="s">
-        <v>3169</v>
+        <v>3171</v>
       </c>
       <c r="D569" s="4" t="s">
-        <v>3170</v>
+        <v>3172</v>
       </c>
       <c r="E569" s="25" t="s">
         <v>1520</v>
@@ -37194,16 +37194,16 @@
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A570" s="4" t="s">
-        <v>3171</v>
+        <v>3173</v>
       </c>
       <c r="B570" s="4" t="s">
-        <v>3172</v>
+        <v>3174</v>
       </c>
       <c r="C570" s="4" t="s">
-        <v>3173</v>
+        <v>3175</v>
       </c>
       <c r="D570" s="4" t="s">
-        <v>3174</v>
+        <v>3176</v>
       </c>
       <c r="E570" s="25" t="s">
         <v>1520</v>
@@ -37211,16 +37211,16 @@
     </row>
     <row r="571" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A571" s="4" t="s">
-        <v>3175</v>
+        <v>3177</v>
       </c>
       <c r="B571" s="4" t="s">
-        <v>3176</v>
+        <v>3178</v>
       </c>
       <c r="C571" s="4" t="s">
-        <v>3177</v>
+        <v>3179</v>
       </c>
       <c r="D571" s="4" t="s">
-        <v>3178</v>
+        <v>3180</v>
       </c>
       <c r="E571" s="25" t="s">
         <v>1520</v>
@@ -37228,16 +37228,16 @@
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A572" s="4" t="s">
-        <v>3179</v>
+        <v>3181</v>
       </c>
       <c r="B572" s="4" t="s">
-        <v>3180</v>
+        <v>3182</v>
       </c>
       <c r="C572" s="4" t="s">
-        <v>3181</v>
+        <v>3183</v>
       </c>
       <c r="D572" s="4" t="s">
-        <v>3182</v>
+        <v>3184</v>
       </c>
       <c r="E572" s="25" t="s">
         <v>1520</v>
@@ -37245,16 +37245,16 @@
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A573" s="4" t="s">
-        <v>3183</v>
+        <v>3185</v>
       </c>
       <c r="B573" s="4" t="s">
-        <v>3184</v>
+        <v>3186</v>
       </c>
       <c r="C573" s="4" t="s">
-        <v>3185</v>
+        <v>3187</v>
       </c>
       <c r="D573" s="4" t="s">
-        <v>3186</v>
+        <v>3188</v>
       </c>
       <c r="E573" s="25" t="s">
         <v>1520</v>
@@ -37262,16 +37262,16 @@
     </row>
     <row r="574" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A574" s="4" t="s">
-        <v>3187</v>
+        <v>3189</v>
       </c>
       <c r="B574" s="4" t="s">
-        <v>3188</v>
+        <v>3190</v>
       </c>
       <c r="C574" s="4" t="s">
-        <v>3189</v>
+        <v>3191</v>
       </c>
       <c r="D574" s="4" t="s">
-        <v>3190</v>
+        <v>3192</v>
       </c>
       <c r="E574" s="25" t="s">
         <v>1520</v>
@@ -37279,16 +37279,16 @@
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A575" s="4" t="s">
-        <v>3191</v>
+        <v>3193</v>
       </c>
       <c r="B575" s="4" t="s">
-        <v>3192</v>
+        <v>3194</v>
       </c>
       <c r="C575" s="4" t="s">
-        <v>3193</v>
+        <v>3195</v>
       </c>
       <c r="D575" s="4" t="s">
-        <v>3194</v>
+        <v>3196</v>
       </c>
       <c r="E575" s="25" t="s">
         <v>1520</v>
@@ -37296,16 +37296,16 @@
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A576" s="4" t="s">
-        <v>3195</v>
+        <v>3197</v>
       </c>
       <c r="B576" s="4" t="s">
-        <v>3196</v>
+        <v>3198</v>
       </c>
       <c r="C576" s="4" t="s">
-        <v>3197</v>
+        <v>3031</v>
       </c>
       <c r="D576" s="4" t="s">
-        <v>3198</v>
+        <v>3199</v>
       </c>
       <c r="E576" s="25" t="s">
         <v>1520</v>
@@ -37313,16 +37313,16 @@
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A577" s="4" t="s">
-        <v>3199</v>
+        <v>3200</v>
       </c>
       <c r="B577" s="4" t="s">
-        <v>3200</v>
+        <v>3201</v>
       </c>
       <c r="C577" s="4" t="s">
-        <v>3031</v>
+        <v>3202</v>
       </c>
       <c r="D577" s="4" t="s">
-        <v>3201</v>
+        <v>3203</v>
       </c>
       <c r="E577" s="25" t="s">
         <v>1520</v>
@@ -37330,16 +37330,16 @@
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A578" s="4" t="s">
-        <v>3202</v>
+        <v>3204</v>
       </c>
       <c r="B578" s="4" t="s">
-        <v>3203</v>
+        <v>3205</v>
       </c>
       <c r="C578" s="4" t="s">
-        <v>3204</v>
+        <v>3206</v>
       </c>
       <c r="D578" s="4" t="s">
-        <v>3205</v>
+        <v>3207</v>
       </c>
       <c r="E578" s="25" t="s">
         <v>1520</v>
@@ -37347,16 +37347,16 @@
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A579" s="4" t="s">
-        <v>3206</v>
+        <v>3208</v>
       </c>
       <c r="B579" s="4" t="s">
-        <v>3207</v>
+        <v>3209</v>
       </c>
       <c r="C579" s="4" t="s">
-        <v>3208</v>
+        <v>3210</v>
       </c>
       <c r="D579" s="4" t="s">
-        <v>3209</v>
+        <v>3211</v>
       </c>
       <c r="E579" s="25" t="s">
         <v>1520</v>
@@ -37364,16 +37364,16 @@
     </row>
     <row r="580" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A580" s="4" t="s">
-        <v>3210</v>
+        <v>3212</v>
       </c>
       <c r="B580" s="4" t="s">
-        <v>3211</v>
+        <v>3213</v>
       </c>
       <c r="C580" s="4" t="s">
-        <v>3212</v>
+        <v>3214</v>
       </c>
       <c r="D580" s="4" t="s">
-        <v>3213</v>
+        <v>3215</v>
       </c>
       <c r="E580" s="25" t="s">
         <v>1520</v>
@@ -37381,16 +37381,16 @@
     </row>
     <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A581" s="4" t="s">
-        <v>3214</v>
+        <v>3216</v>
       </c>
       <c r="B581" s="4" t="s">
-        <v>3215</v>
+        <v>3217</v>
       </c>
       <c r="C581" s="4" t="s">
-        <v>3216</v>
+        <v>3218</v>
       </c>
       <c r="D581" s="4" t="s">
-        <v>3217</v>
+        <v>3219</v>
       </c>
       <c r="E581" s="25" t="s">
         <v>1520</v>
@@ -37398,16 +37398,16 @@
     </row>
     <row r="582" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A582" s="4" t="s">
-        <v>3218</v>
+        <v>3220</v>
       </c>
       <c r="B582" s="4" t="s">
-        <v>3219</v>
+        <v>3221</v>
       </c>
       <c r="C582" s="4" t="s">
-        <v>3220</v>
+        <v>3222</v>
       </c>
       <c r="D582" s="4" t="s">
-        <v>3221</v>
+        <v>3223</v>
       </c>
       <c r="E582" s="25" t="s">
         <v>1520</v>
@@ -37415,16 +37415,16 @@
     </row>
     <row r="583" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A583" s="4" t="s">
-        <v>3222</v>
+        <v>3224</v>
       </c>
       <c r="B583" s="4" t="s">
-        <v>3223</v>
+        <v>3225</v>
       </c>
       <c r="C583" s="4" t="s">
-        <v>3224</v>
+        <v>3226</v>
       </c>
       <c r="D583" s="4" t="s">
-        <v>3225</v>
+        <v>3227</v>
       </c>
       <c r="E583" s="25" t="s">
         <v>1520</v>
@@ -37432,16 +37432,16 @@
     </row>
     <row r="584" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A584" s="4" t="s">
-        <v>3226</v>
+        <v>3228</v>
       </c>
       <c r="B584" s="4" t="s">
-        <v>3227</v>
+        <v>3229</v>
       </c>
       <c r="C584" s="4" t="s">
-        <v>3228</v>
+        <v>3230</v>
       </c>
       <c r="D584" s="4" t="s">
-        <v>3229</v>
+        <v>3231</v>
       </c>
       <c r="E584" s="25" t="s">
         <v>1520</v>
@@ -37449,16 +37449,16 @@
     </row>
     <row r="585" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A585" s="4" t="s">
-        <v>3230</v>
+        <v>3232</v>
       </c>
       <c r="B585" s="4" t="s">
-        <v>3231</v>
+        <v>3233</v>
       </c>
       <c r="C585" s="4" t="s">
-        <v>3232</v>
+        <v>3234</v>
       </c>
       <c r="D585" s="4" t="s">
-        <v>3233</v>
+        <v>3235</v>
       </c>
       <c r="E585" s="25" t="s">
         <v>1520</v>
@@ -37466,16 +37466,16 @@
     </row>
     <row r="586" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A586" s="4" t="s">
-        <v>3234</v>
+        <v>3236</v>
       </c>
       <c r="B586" s="4" t="s">
-        <v>3235</v>
+        <v>3237</v>
       </c>
       <c r="C586" s="4" t="s">
-        <v>3236</v>
+        <v>3238</v>
       </c>
       <c r="D586" s="4" t="s">
-        <v>3237</v>
+        <v>3239</v>
       </c>
       <c r="E586" s="25" t="s">
         <v>1520</v>
@@ -37483,16 +37483,16 @@
     </row>
     <row r="587" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A587" s="4" t="s">
-        <v>3238</v>
+        <v>3240</v>
       </c>
       <c r="B587" s="4" t="s">
-        <v>3239</v>
+        <v>3241</v>
       </c>
       <c r="C587" s="4" t="s">
-        <v>3240</v>
+        <v>3242</v>
       </c>
       <c r="D587" s="4" t="s">
-        <v>3241</v>
+        <v>1668</v>
       </c>
       <c r="E587" s="25" t="s">
         <v>1520</v>
@@ -37500,16 +37500,16 @@
     </row>
     <row r="588" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A588" s="4" t="s">
-        <v>3242</v>
+        <v>3243</v>
       </c>
       <c r="B588" s="4" t="s">
-        <v>3243</v>
+        <v>3244</v>
       </c>
       <c r="C588" s="4" t="s">
-        <v>3244</v>
+        <v>3245</v>
       </c>
       <c r="D588" s="4" t="s">
-        <v>1668</v>
+        <v>3246</v>
       </c>
       <c r="E588" s="25" t="s">
         <v>1520</v>
@@ -37517,16 +37517,16 @@
     </row>
     <row r="589" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A589" s="4" t="s">
-        <v>3245</v>
+        <v>3247</v>
       </c>
       <c r="B589" s="4" t="s">
-        <v>3246</v>
+        <v>3248</v>
       </c>
       <c r="C589" s="4" t="s">
-        <v>3247</v>
+        <v>3249</v>
       </c>
       <c r="D589" s="4" t="s">
-        <v>3248</v>
+        <v>3250</v>
       </c>
       <c r="E589" s="25" t="s">
         <v>1520</v>
@@ -37534,16 +37534,16 @@
     </row>
     <row r="590" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A590" s="4" t="s">
-        <v>3249</v>
+        <v>3251</v>
       </c>
       <c r="B590" s="4" t="s">
-        <v>3250</v>
+        <v>3252</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>3251</v>
+        <v>3253</v>
       </c>
       <c r="D590" s="4" t="s">
-        <v>3252</v>
+        <v>3254</v>
       </c>
       <c r="E590" s="25" t="s">
         <v>1520</v>
@@ -37551,16 +37551,16 @@
     </row>
     <row r="591" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A591" s="4" t="s">
-        <v>3253</v>
+        <v>3255</v>
       </c>
       <c r="B591" s="4" t="s">
-        <v>3254</v>
+        <v>3256</v>
       </c>
       <c r="C591" s="4" t="s">
-        <v>3255</v>
+        <v>3257</v>
       </c>
       <c r="D591" s="4" t="s">
-        <v>3256</v>
+        <v>3258</v>
       </c>
       <c r="E591" s="25" t="s">
         <v>1520</v>
@@ -37568,16 +37568,16 @@
     </row>
     <row r="592" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A592" s="4" t="s">
-        <v>3257</v>
+        <v>3259</v>
       </c>
       <c r="B592" s="4" t="s">
-        <v>3258</v>
+        <v>3260</v>
       </c>
       <c r="C592" s="4" t="s">
-        <v>3259</v>
+        <v>3261</v>
       </c>
       <c r="D592" s="4" t="s">
-        <v>3260</v>
+        <v>3262</v>
       </c>
       <c r="E592" s="25" t="s">
         <v>1520</v>
@@ -37585,16 +37585,16 @@
     </row>
     <row r="593" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A593" s="4" t="s">
-        <v>3261</v>
+        <v>3263</v>
       </c>
       <c r="B593" s="4" t="s">
-        <v>3262</v>
+        <v>3264</v>
       </c>
       <c r="C593" s="4" t="s">
-        <v>3263</v>
+        <v>3265</v>
       </c>
       <c r="D593" s="4" t="s">
-        <v>3264</v>
+        <v>3266</v>
       </c>
       <c r="E593" s="25" t="s">
         <v>1520</v>
@@ -37602,16 +37602,16 @@
     </row>
     <row r="594" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A594" s="4" t="s">
-        <v>3265</v>
+        <v>3267</v>
       </c>
       <c r="B594" s="4" t="s">
-        <v>3266</v>
+        <v>3268</v>
       </c>
       <c r="C594" s="4" t="s">
-        <v>3267</v>
+        <v>3269</v>
       </c>
       <c r="D594" s="4" t="s">
-        <v>3268</v>
+        <v>3270</v>
       </c>
       <c r="E594" s="25" t="s">
         <v>1520</v>
@@ -37619,16 +37619,16 @@
     </row>
     <row r="595" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A595" s="4" t="s">
-        <v>3269</v>
+        <v>3271</v>
       </c>
       <c r="B595" s="4" t="s">
-        <v>3270</v>
+        <v>3272</v>
       </c>
       <c r="C595" s="4" t="s">
-        <v>3271</v>
+        <v>3273</v>
       </c>
       <c r="D595" s="4" t="s">
-        <v>3272</v>
+        <v>3274</v>
       </c>
       <c r="E595" s="25" t="s">
         <v>1520</v>
@@ -37636,16 +37636,16 @@
     </row>
     <row r="596" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A596" s="4" t="s">
-        <v>3273</v>
+        <v>3275</v>
       </c>
       <c r="B596" s="4" t="s">
-        <v>3274</v>
+        <v>3276</v>
       </c>
       <c r="C596" s="4" t="s">
-        <v>3275</v>
+        <v>3277</v>
       </c>
       <c r="D596" s="4" t="s">
-        <v>3276</v>
+        <v>3278</v>
       </c>
       <c r="E596" s="25" t="s">
         <v>1520</v>
@@ -37653,16 +37653,16 @@
     </row>
     <row r="597" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A597" s="4" t="s">
-        <v>3277</v>
+        <v>3279</v>
       </c>
       <c r="B597" s="4" t="s">
-        <v>3278</v>
+        <v>3280</v>
       </c>
       <c r="C597" s="4" t="s">
-        <v>3279</v>
+        <v>3281</v>
       </c>
       <c r="D597" s="4" t="s">
-        <v>3280</v>
+        <v>3282</v>
       </c>
       <c r="E597" s="25" t="s">
         <v>1520</v>
@@ -37670,16 +37670,16 @@
     </row>
     <row r="598" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A598" s="4" t="s">
-        <v>3281</v>
+        <v>3283</v>
       </c>
       <c r="B598" s="4" t="s">
-        <v>3282</v>
+        <v>3284</v>
       </c>
       <c r="C598" s="4" t="s">
-        <v>3283</v>
+        <v>3285</v>
       </c>
       <c r="D598" s="4" t="s">
-        <v>3284</v>
+        <v>3286</v>
       </c>
       <c r="E598" s="25" t="s">
         <v>1520</v>
@@ -37687,16 +37687,16 @@
     </row>
     <row r="599" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A599" s="4" t="s">
-        <v>3285</v>
+        <v>3287</v>
       </c>
       <c r="B599" s="4" t="s">
-        <v>3286</v>
+        <v>3288</v>
       </c>
       <c r="C599" s="4" t="s">
-        <v>3287</v>
+        <v>3289</v>
       </c>
       <c r="D599" s="4" t="s">
-        <v>3288</v>
+        <v>3290</v>
       </c>
       <c r="E599" s="25" t="s">
         <v>1520</v>
@@ -37704,16 +37704,16 @@
     </row>
     <row r="600" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A600" s="4" t="s">
-        <v>3289</v>
+        <v>3291</v>
       </c>
       <c r="B600" s="4" t="s">
-        <v>3290</v>
+        <v>3292</v>
       </c>
       <c r="C600" s="4" t="s">
-        <v>3291</v>
+        <v>3293</v>
       </c>
       <c r="D600" s="4" t="s">
-        <v>3292</v>
+        <v>3294</v>
       </c>
       <c r="E600" s="25" t="s">
         <v>1520</v>
@@ -37721,16 +37721,16 @@
     </row>
     <row r="601" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A601" s="4" t="s">
-        <v>3293</v>
+        <v>3295</v>
       </c>
       <c r="B601" s="4" t="s">
-        <v>3294</v>
+        <v>3296</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>3295</v>
+        <v>3297</v>
       </c>
       <c r="D601" s="4" t="s">
-        <v>3296</v>
+        <v>3298</v>
       </c>
       <c r="E601" s="25" t="s">
         <v>1520</v>
@@ -37738,16 +37738,16 @@
     </row>
     <row r="602" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A602" s="4" t="s">
-        <v>3297</v>
+        <v>3299</v>
       </c>
       <c r="B602" s="4" t="s">
-        <v>3298</v>
+        <v>3300</v>
       </c>
       <c r="C602" s="4" t="s">
-        <v>3299</v>
+        <v>3301</v>
       </c>
       <c r="D602" s="4" t="s">
-        <v>3300</v>
+        <v>3302</v>
       </c>
       <c r="E602" s="25" t="s">
         <v>1520</v>
@@ -37755,16 +37755,16 @@
     </row>
     <row r="603" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A603" s="4" t="s">
-        <v>3301</v>
+        <v>3303</v>
       </c>
       <c r="B603" s="4" t="s">
-        <v>3302</v>
+        <v>3304</v>
       </c>
       <c r="C603" s="4" t="s">
-        <v>3303</v>
+        <v>3305</v>
       </c>
       <c r="D603" s="4" t="s">
-        <v>3304</v>
+        <v>3306</v>
       </c>
       <c r="E603" s="25" t="s">
         <v>1520</v>
@@ -37772,16 +37772,16 @@
     </row>
     <row r="604" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A604" s="4" t="s">
-        <v>3305</v>
+        <v>3307</v>
       </c>
       <c r="B604" s="4" t="s">
-        <v>3306</v>
+        <v>3308</v>
       </c>
       <c r="C604" s="4" t="s">
-        <v>3307</v>
+        <v>3309</v>
       </c>
       <c r="D604" s="4" t="s">
-        <v>3308</v>
+        <v>3310</v>
       </c>
       <c r="E604" s="25" t="s">
         <v>1520</v>
@@ -37789,16 +37789,16 @@
     </row>
     <row r="605" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A605" s="4" t="s">
-        <v>3309</v>
+        <v>3311</v>
       </c>
       <c r="B605" s="4" t="s">
-        <v>3310</v>
+        <v>3312</v>
       </c>
       <c r="C605" s="4" t="s">
-        <v>3311</v>
+        <v>3313</v>
       </c>
       <c r="D605" s="4" t="s">
-        <v>3312</v>
+        <v>3314</v>
       </c>
       <c r="E605" s="25" t="s">
         <v>1520</v>
@@ -37806,16 +37806,16 @@
     </row>
     <row r="606" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A606" s="4" t="s">
-        <v>3313</v>
+        <v>3315</v>
       </c>
       <c r="B606" s="4" t="s">
-        <v>3314</v>
+        <v>3316</v>
       </c>
       <c r="C606" s="4" t="s">
-        <v>3315</v>
+        <v>3317</v>
       </c>
       <c r="D606" s="4" t="s">
-        <v>3316</v>
+        <v>3318</v>
       </c>
       <c r="E606" s="25" t="s">
         <v>1520</v>
@@ -37823,16 +37823,16 @@
     </row>
     <row r="607" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A607" s="4" t="s">
-        <v>3317</v>
+        <v>3319</v>
       </c>
       <c r="B607" s="4" t="s">
-        <v>3318</v>
+        <v>3320</v>
       </c>
       <c r="C607" s="4" t="s">
-        <v>3319</v>
+        <v>3321</v>
       </c>
       <c r="D607" s="4" t="s">
-        <v>3320</v>
+        <v>3322</v>
       </c>
       <c r="E607" s="25" t="s">
         <v>1520</v>
@@ -37840,16 +37840,16 @@
     </row>
     <row r="608" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A608" s="4" t="s">
-        <v>3321</v>
+        <v>3323</v>
       </c>
       <c r="B608" s="4" t="s">
-        <v>3322</v>
+        <v>3324</v>
       </c>
       <c r="C608" s="4" t="s">
-        <v>3323</v>
+        <v>3325</v>
       </c>
       <c r="D608" s="4" t="s">
-        <v>3324</v>
+        <v>3326</v>
       </c>
       <c r="E608" s="25" t="s">
         <v>1520</v>
@@ -37857,16 +37857,16 @@
     </row>
     <row r="609" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A609" s="4" t="s">
-        <v>3325</v>
+        <v>3327</v>
       </c>
       <c r="B609" s="4" t="s">
-        <v>3326</v>
+        <v>3328</v>
       </c>
       <c r="C609" s="4" t="s">
-        <v>3327</v>
+        <v>3329</v>
       </c>
       <c r="D609" s="4" t="s">
-        <v>3328</v>
+        <v>3330</v>
       </c>
       <c r="E609" s="25" t="s">
         <v>1520</v>
@@ -37874,16 +37874,16 @@
     </row>
     <row r="610" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A610" s="4" t="s">
-        <v>3329</v>
+        <v>3331</v>
       </c>
       <c r="B610" s="4" t="s">
-        <v>3330</v>
+        <v>3332</v>
       </c>
       <c r="C610" s="4" t="s">
-        <v>3331</v>
+        <v>3333</v>
       </c>
       <c r="D610" s="4" t="s">
-        <v>3332</v>
+        <v>3334</v>
       </c>
       <c r="E610" s="25" t="s">
         <v>1520</v>
@@ -37891,16 +37891,16 @@
     </row>
     <row r="611" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A611" s="4" t="s">
-        <v>3333</v>
+        <v>3335</v>
       </c>
       <c r="B611" s="4" t="s">
-        <v>3334</v>
+        <v>3336</v>
       </c>
       <c r="C611" s="4" t="s">
-        <v>3335</v>
+        <v>3337</v>
       </c>
       <c r="D611" s="4" t="s">
-        <v>3336</v>
+        <v>3338</v>
       </c>
       <c r="E611" s="25" t="s">
         <v>1520</v>
@@ -37908,16 +37908,16 @@
     </row>
     <row r="612" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A612" s="4" t="s">
-        <v>3337</v>
+        <v>3339</v>
       </c>
       <c r="B612" s="4" t="s">
-        <v>3338</v>
+        <v>3340</v>
       </c>
       <c r="C612" s="4" t="s">
-        <v>3339</v>
+        <v>3341</v>
       </c>
       <c r="D612" s="4" t="s">
-        <v>3340</v>
+        <v>3342</v>
       </c>
       <c r="E612" s="25" t="s">
         <v>1520</v>
@@ -37925,16 +37925,16 @@
     </row>
     <row r="613" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A613" s="4" t="s">
-        <v>3341</v>
+        <v>3343</v>
       </c>
       <c r="B613" s="4" t="s">
-        <v>3342</v>
+        <v>3344</v>
       </c>
       <c r="C613" s="4" t="s">
-        <v>3343</v>
+        <v>3345</v>
       </c>
       <c r="D613" s="4" t="s">
-        <v>3344</v>
+        <v>3346</v>
       </c>
       <c r="E613" s="25" t="s">
         <v>1520</v>
@@ -37942,16 +37942,16 @@
     </row>
     <row r="614" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A614" s="4" t="s">
-        <v>3345</v>
+        <v>3347</v>
       </c>
       <c r="B614" s="4" t="s">
-        <v>3346</v>
+        <v>3348</v>
       </c>
       <c r="C614" s="4" t="s">
-        <v>3347</v>
+        <v>3349</v>
       </c>
       <c r="D614" s="4" t="s">
-        <v>3348</v>
+        <v>3350</v>
       </c>
       <c r="E614" s="25" t="s">
         <v>1520</v>
@@ -37959,16 +37959,16 @@
     </row>
     <row r="615" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A615" s="4" t="s">
-        <v>3349</v>
+        <v>3351</v>
       </c>
       <c r="B615" s="4" t="s">
-        <v>3350</v>
+        <v>3352</v>
       </c>
       <c r="C615" s="4" t="s">
-        <v>3351</v>
+        <v>3353</v>
       </c>
       <c r="D615" s="4" t="s">
-        <v>3352</v>
+        <v>3354</v>
       </c>
       <c r="E615" s="25" t="s">
         <v>1520</v>
@@ -37976,16 +37976,16 @@
     </row>
     <row r="616" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A616" s="4" t="s">
-        <v>3353</v>
+        <v>3355</v>
       </c>
       <c r="B616" s="4" t="s">
-        <v>3354</v>
+        <v>3356</v>
       </c>
       <c r="C616" s="4" t="s">
-        <v>3355</v>
+        <v>3357</v>
       </c>
       <c r="D616" s="4" t="s">
-        <v>3356</v>
+        <v>1752</v>
       </c>
       <c r="E616" s="25" t="s">
         <v>1520</v>
@@ -37993,16 +37993,16 @@
     </row>
     <row r="617" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A617" s="4" t="s">
-        <v>3357</v>
+        <v>3358</v>
       </c>
       <c r="B617" s="4" t="s">
-        <v>3358</v>
+        <v>3359</v>
       </c>
       <c r="C617" s="4" t="s">
-        <v>3359</v>
+        <v>3360</v>
       </c>
       <c r="D617" s="4" t="s">
-        <v>1752</v>
+        <v>3361</v>
       </c>
       <c r="E617" s="25" t="s">
         <v>1520</v>
@@ -38010,13 +38010,13 @@
     </row>
     <row r="618" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A618" s="4" t="s">
-        <v>3360</v>
+        <v>3362</v>
       </c>
       <c r="B618" s="4" t="s">
-        <v>3361</v>
+        <v>3363</v>
       </c>
       <c r="C618" s="4" t="s">
-        <v>3362</v>
+        <v>3363</v>
       </c>
       <c r="D618" s="4" t="s">
         <v>3363</v>
@@ -38033,10 +38033,10 @@
         <v>3365</v>
       </c>
       <c r="C619" s="4" t="s">
-        <v>3365</v>
+        <v>3366</v>
       </c>
       <c r="D619" s="4" t="s">
-        <v>3365</v>
+        <v>3367</v>
       </c>
       <c r="E619" s="25" t="s">
         <v>1520</v>
@@ -38044,16 +38044,16 @@
     </row>
     <row r="620" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A620" s="4" t="s">
-        <v>3366</v>
+        <v>3368</v>
       </c>
       <c r="B620" s="4" t="s">
-        <v>3367</v>
+        <v>3369</v>
       </c>
       <c r="C620" s="4" t="s">
-        <v>3368</v>
+        <v>3370</v>
       </c>
       <c r="D620" s="4" t="s">
-        <v>3369</v>
+        <v>3371</v>
       </c>
       <c r="E620" s="25" t="s">
         <v>1520</v>
@@ -38061,16 +38061,16 @@
     </row>
     <row r="621" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A621" s="4" t="s">
-        <v>3370</v>
+        <v>3372</v>
       </c>
       <c r="B621" s="4" t="s">
-        <v>3371</v>
+        <v>3373</v>
       </c>
       <c r="C621" s="4" t="s">
-        <v>3372</v>
+        <v>3374</v>
       </c>
       <c r="D621" s="4" t="s">
-        <v>3373</v>
+        <v>3375</v>
       </c>
       <c r="E621" s="25" t="s">
         <v>1520</v>
@@ -38078,16 +38078,16 @@
     </row>
     <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A622" s="4" t="s">
-        <v>3374</v>
+        <v>3376</v>
       </c>
       <c r="B622" s="4" t="s">
-        <v>3375</v>
+        <v>3377</v>
       </c>
       <c r="C622" s="4" t="s">
-        <v>3376</v>
+        <v>3378</v>
       </c>
       <c r="D622" s="4" t="s">
-        <v>3377</v>
+        <v>3379</v>
       </c>
       <c r="E622" s="25" t="s">
         <v>1520</v>
@@ -38095,16 +38095,16 @@
     </row>
     <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A623" s="4" t="s">
-        <v>3378</v>
+        <v>3380</v>
       </c>
       <c r="B623" s="4" t="s">
-        <v>3379</v>
+        <v>3381</v>
       </c>
       <c r="C623" s="4" t="s">
-        <v>3380</v>
+        <v>3382</v>
       </c>
       <c r="D623" s="4" t="s">
-        <v>3381</v>
+        <v>3383</v>
       </c>
       <c r="E623" s="25" t="s">
         <v>1520</v>
@@ -38112,16 +38112,16 @@
     </row>
     <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A624" s="4" t="s">
-        <v>3382</v>
+        <v>3384</v>
       </c>
       <c r="B624" s="4" t="s">
-        <v>3383</v>
+        <v>3385</v>
       </c>
       <c r="C624" s="4" t="s">
-        <v>3384</v>
+        <v>3386</v>
       </c>
       <c r="D624" s="4" t="s">
-        <v>3385</v>
+        <v>3387</v>
       </c>
       <c r="E624" s="25" t="s">
         <v>1520</v>
@@ -38129,16 +38129,16 @@
     </row>
     <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A625" s="4" t="s">
-        <v>3386</v>
+        <v>3388</v>
       </c>
       <c r="B625" s="4" t="s">
-        <v>3387</v>
+        <v>3389</v>
       </c>
       <c r="C625" s="4" t="s">
-        <v>3388</v>
+        <v>3390</v>
       </c>
       <c r="D625" s="4" t="s">
-        <v>3389</v>
+        <v>3391</v>
       </c>
       <c r="E625" s="25" t="s">
         <v>1520</v>
@@ -38146,16 +38146,16 @@
     </row>
     <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A626" s="4" t="s">
-        <v>3390</v>
+        <v>3392</v>
       </c>
       <c r="B626" s="4" t="s">
-        <v>3391</v>
+        <v>3393</v>
       </c>
       <c r="C626" s="4" t="s">
-        <v>3392</v>
+        <v>3394</v>
       </c>
       <c r="D626" s="4" t="s">
-        <v>3393</v>
+        <v>3395</v>
       </c>
       <c r="E626" s="25" t="s">
         <v>1520</v>
@@ -38163,16 +38163,16 @@
     </row>
     <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A627" s="4" t="s">
-        <v>3394</v>
+        <v>3396</v>
       </c>
       <c r="B627" s="4" t="s">
-        <v>3395</v>
+        <v>3397</v>
       </c>
       <c r="C627" s="4" t="s">
-        <v>3396</v>
+        <v>3398</v>
       </c>
       <c r="D627" s="4" t="s">
-        <v>3397</v>
+        <v>3399</v>
       </c>
       <c r="E627" s="25" t="s">
         <v>1520</v>
@@ -38180,16 +38180,16 @@
     </row>
     <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A628" s="4" t="s">
-        <v>3398</v>
+        <v>3400</v>
       </c>
       <c r="B628" s="4" t="s">
-        <v>3399</v>
+        <v>3401</v>
       </c>
       <c r="C628" s="4" t="s">
-        <v>3400</v>
+        <v>3402</v>
       </c>
       <c r="D628" s="4" t="s">
-        <v>3401</v>
+        <v>3403</v>
       </c>
       <c r="E628" s="25" t="s">
         <v>1520</v>
@@ -38197,16 +38197,16 @@
     </row>
     <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A629" s="4" t="s">
-        <v>3402</v>
+        <v>3404</v>
       </c>
       <c r="B629" s="4" t="s">
-        <v>3403</v>
+        <v>3405</v>
       </c>
       <c r="C629" s="4" t="s">
-        <v>3404</v>
+        <v>3406</v>
       </c>
       <c r="D629" s="4" t="s">
-        <v>3405</v>
+        <v>1710</v>
       </c>
       <c r="E629" s="25" t="s">
         <v>1520</v>
@@ -38214,16 +38214,16 @@
     </row>
     <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A630" s="4" t="s">
-        <v>3406</v>
+        <v>3407</v>
       </c>
       <c r="B630" s="4" t="s">
-        <v>3407</v>
+        <v>3408</v>
       </c>
       <c r="C630" s="4" t="s">
-        <v>3408</v>
+        <v>3409</v>
       </c>
       <c r="D630" s="4" t="s">
-        <v>1710</v>
+        <v>3410</v>
       </c>
       <c r="E630" s="25" t="s">
         <v>1520</v>
@@ -38231,16 +38231,16 @@
     </row>
     <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A631" s="4" t="s">
-        <v>3409</v>
+        <v>3411</v>
       </c>
       <c r="B631" s="4" t="s">
-        <v>3410</v>
+        <v>3412</v>
       </c>
       <c r="C631" s="4" t="s">
-        <v>3411</v>
+        <v>3413</v>
       </c>
       <c r="D631" s="4" t="s">
-        <v>3412</v>
+        <v>3414</v>
       </c>
       <c r="E631" s="25" t="s">
         <v>1520</v>
@@ -38248,16 +38248,16 @@
     </row>
     <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A632" s="4" t="s">
-        <v>3413</v>
+        <v>3415</v>
       </c>
       <c r="B632" s="4" t="s">
-        <v>3414</v>
+        <v>3416</v>
       </c>
       <c r="C632" s="4" t="s">
-        <v>3415</v>
+        <v>3417</v>
       </c>
       <c r="D632" s="4" t="s">
-        <v>3416</v>
+        <v>3418</v>
       </c>
       <c r="E632" s="25" t="s">
         <v>1520</v>
@@ -38265,16 +38265,16 @@
     </row>
     <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A633" s="4" t="s">
-        <v>3417</v>
+        <v>3419</v>
       </c>
       <c r="B633" s="4" t="s">
-        <v>3418</v>
+        <v>3420</v>
       </c>
       <c r="C633" s="4" t="s">
-        <v>3419</v>
+        <v>3421</v>
       </c>
       <c r="D633" s="4" t="s">
-        <v>3420</v>
+        <v>3422</v>
       </c>
       <c r="E633" s="25" t="s">
         <v>1520</v>
@@ -38282,16 +38282,16 @@
     </row>
     <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A634" s="4" t="s">
-        <v>3421</v>
+        <v>3423</v>
       </c>
       <c r="B634" s="4" t="s">
-        <v>3422</v>
+        <v>3424</v>
       </c>
       <c r="C634" s="4" t="s">
-        <v>3423</v>
+        <v>3425</v>
       </c>
       <c r="D634" s="4" t="s">
-        <v>3424</v>
+        <v>3426</v>
       </c>
       <c r="E634" s="25" t="s">
         <v>1520</v>
@@ -38299,16 +38299,16 @@
     </row>
     <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A635" s="4" t="s">
-        <v>3425</v>
+        <v>3427</v>
       </c>
       <c r="B635" s="4" t="s">
-        <v>3426</v>
+        <v>3428</v>
       </c>
       <c r="C635" s="4" t="s">
-        <v>3427</v>
+        <v>3429</v>
       </c>
       <c r="D635" s="4" t="s">
-        <v>3428</v>
+        <v>3430</v>
       </c>
       <c r="E635" s="25" t="s">
         <v>1520</v>
@@ -38316,16 +38316,16 @@
     </row>
     <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A636" s="4" t="s">
-        <v>3429</v>
+        <v>3431</v>
       </c>
       <c r="B636" s="4" t="s">
-        <v>3430</v>
+        <v>3432</v>
       </c>
       <c r="C636" s="4" t="s">
-        <v>3431</v>
+        <v>3433</v>
       </c>
       <c r="D636" s="4" t="s">
-        <v>3432</v>
+        <v>3434</v>
       </c>
       <c r="E636" s="25" t="s">
         <v>1520</v>
@@ -38333,16 +38333,16 @@
     </row>
     <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A637" s="4" t="s">
-        <v>3433</v>
+        <v>3435</v>
       </c>
       <c r="B637" s="4" t="s">
-        <v>3434</v>
+        <v>3436</v>
       </c>
       <c r="C637" s="4" t="s">
-        <v>3435</v>
+        <v>3437</v>
       </c>
       <c r="D637" s="4" t="s">
-        <v>3436</v>
+        <v>3438</v>
       </c>
       <c r="E637" s="25" t="s">
         <v>1520</v>
@@ -38350,16 +38350,16 @@
     </row>
     <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A638" s="4" t="s">
-        <v>3437</v>
+        <v>3439</v>
       </c>
       <c r="B638" s="4" t="s">
-        <v>3438</v>
+        <v>3440</v>
       </c>
       <c r="C638" s="4" t="s">
-        <v>3439</v>
+        <v>3441</v>
       </c>
       <c r="D638" s="4" t="s">
-        <v>3440</v>
+        <v>3442</v>
       </c>
       <c r="E638" s="25" t="s">
         <v>1520</v>
@@ -38367,16 +38367,16 @@
     </row>
     <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A639" s="4" t="s">
-        <v>3441</v>
+        <v>3443</v>
       </c>
       <c r="B639" s="4" t="s">
-        <v>3442</v>
+        <v>3444</v>
       </c>
       <c r="C639" s="4" t="s">
-        <v>3443</v>
+        <v>3445</v>
       </c>
       <c r="D639" s="4" t="s">
-        <v>3444</v>
+        <v>3446</v>
       </c>
       <c r="E639" s="25" t="s">
         <v>1520</v>
@@ -38384,16 +38384,16 @@
     </row>
     <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A640" s="4" t="s">
-        <v>3445</v>
+        <v>3447</v>
       </c>
       <c r="B640" s="4" t="s">
-        <v>3446</v>
+        <v>3448</v>
       </c>
       <c r="C640" s="4" t="s">
-        <v>3447</v>
+        <v>3449</v>
       </c>
       <c r="D640" s="4" t="s">
-        <v>3448</v>
+        <v>3450</v>
       </c>
       <c r="E640" s="25" t="s">
         <v>1520</v>
@@ -38401,16 +38401,16 @@
     </row>
     <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A641" s="4" t="s">
-        <v>3449</v>
+        <v>3451</v>
       </c>
       <c r="B641" s="4" t="s">
-        <v>3450</v>
-      </c>
-      <c r="C641" s="1" t="s">
-        <v>3451</v>
+        <v>3452</v>
+      </c>
+      <c r="C641" s="4" t="s">
+        <v>3453</v>
       </c>
       <c r="D641" s="4" t="s">
-        <v>3452</v>
+        <v>3454</v>
       </c>
       <c r="E641" s="25" t="s">
         <v>1520</v>
@@ -38418,16 +38418,16 @@
     </row>
     <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A642" s="4" t="s">
-        <v>3453</v>
+        <v>3455</v>
       </c>
       <c r="B642" s="4" t="s">
-        <v>3454</v>
+        <v>3456</v>
       </c>
       <c r="C642" s="4" t="s">
-        <v>3455</v>
+        <v>3457</v>
       </c>
       <c r="D642" s="4" t="s">
-        <v>3456</v>
+        <v>3458</v>
       </c>
       <c r="E642" s="25" t="s">
         <v>1520</v>
@@ -38435,16 +38435,16 @@
     </row>
     <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A643" s="4" t="s">
-        <v>3457</v>
+        <v>3459</v>
       </c>
       <c r="B643" s="4" t="s">
-        <v>3458</v>
+        <v>3460</v>
       </c>
       <c r="C643" s="4" t="s">
-        <v>3459</v>
+        <v>3461</v>
       </c>
       <c r="D643" s="4" t="s">
-        <v>3460</v>
+        <v>3462</v>
       </c>
       <c r="E643" s="25" t="s">
         <v>1520</v>
@@ -38452,16 +38452,16 @@
     </row>
     <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A644" s="4" t="s">
-        <v>3461</v>
+        <v>3463</v>
       </c>
       <c r="B644" s="4" t="s">
-        <v>3462</v>
+        <v>3464</v>
       </c>
       <c r="C644" s="4" t="s">
-        <v>3463</v>
+        <v>3465</v>
       </c>
       <c r="D644" s="4" t="s">
-        <v>3464</v>
+        <v>3466</v>
       </c>
       <c r="E644" s="25" t="s">
         <v>1520</v>
@@ -38469,16 +38469,16 @@
     </row>
     <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A645" s="4" t="s">
-        <v>3465</v>
+        <v>3467</v>
       </c>
       <c r="B645" s="4" t="s">
-        <v>3466</v>
+        <v>3468</v>
       </c>
       <c r="C645" s="4" t="s">
-        <v>3467</v>
+        <v>3469</v>
       </c>
       <c r="D645" s="4" t="s">
-        <v>3468</v>
+        <v>3470</v>
       </c>
       <c r="E645" s="25" t="s">
         <v>1520</v>
@@ -38486,16 +38486,16 @@
     </row>
     <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A646" s="4" t="s">
-        <v>3469</v>
+        <v>3471</v>
       </c>
       <c r="B646" s="4" t="s">
-        <v>3470</v>
+        <v>3472</v>
       </c>
       <c r="C646" s="4" t="s">
-        <v>3471</v>
+        <v>3473</v>
       </c>
       <c r="D646" s="4" t="s">
-        <v>3472</v>
+        <v>3474</v>
       </c>
       <c r="E646" s="25" t="s">
         <v>1520</v>
@@ -38503,16 +38503,16 @@
     </row>
     <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A647" s="4" t="s">
-        <v>3473</v>
+        <v>3475</v>
       </c>
       <c r="B647" s="4" t="s">
-        <v>3474</v>
+        <v>3476</v>
       </c>
       <c r="C647" s="4" t="s">
-        <v>3475</v>
+        <v>3477</v>
       </c>
       <c r="D647" s="4" t="s">
-        <v>3476</v>
+        <v>3478</v>
       </c>
       <c r="E647" s="25" t="s">
         <v>1520</v>
@@ -38520,16 +38520,16 @@
     </row>
     <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A648" s="4" t="s">
-        <v>3477</v>
+        <v>3479</v>
       </c>
       <c r="B648" s="4" t="s">
-        <v>3478</v>
+        <v>3480</v>
       </c>
       <c r="C648" s="4" t="s">
-        <v>3479</v>
+        <v>3481</v>
       </c>
       <c r="D648" s="4" t="s">
-        <v>3480</v>
+        <v>3482</v>
       </c>
       <c r="E648" s="25" t="s">
         <v>1520</v>
@@ -38537,70 +38537,70 @@
     </row>
     <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A649" s="4" t="s">
-        <v>3481</v>
+        <v>3483</v>
       </c>
       <c r="B649" s="4" t="s">
-        <v>3482</v>
+        <v>3484</v>
       </c>
       <c r="C649" s="4" t="s">
-        <v>3483</v>
+        <v>3485</v>
       </c>
       <c r="D649" s="4" t="s">
-        <v>3484</v>
+        <v>3486</v>
       </c>
       <c r="E649" s="25" t="s">
-        <v>1520</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="4" t="s">
-        <v>3485</v>
+        <v>3487</v>
       </c>
       <c r="B650" s="4" t="s">
-        <v>3486</v>
+        <v>3488</v>
       </c>
       <c r="C650" s="4" t="s">
-        <v>3487</v>
+        <v>3489</v>
       </c>
       <c r="D650" s="4" t="s">
-        <v>3488</v>
+        <v>3490</v>
       </c>
       <c r="E650" s="25" t="s">
-        <v>2014</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="4" t="s">
-        <v>3489</v>
+        <v>3491</v>
       </c>
       <c r="B651" s="4" t="s">
-        <v>3490</v>
+        <v>3492</v>
       </c>
       <c r="C651" s="4" t="s">
-        <v>3491</v>
-      </c>
-      <c r="D651" s="4" t="s">
-        <v>3492</v>
-      </c>
-      <c r="E651" s="25" t="s">
-        <v>2044</v>
+        <v>3493</v>
+      </c>
+      <c r="D651" s="11" t="s">
+        <v>3494</v>
+      </c>
+      <c r="E651" s="26" t="s">
+        <v>2110</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="4" t="s">
-        <v>3493</v>
+        <v>3495</v>
       </c>
       <c r="B652" s="4" t="s">
-        <v>3494</v>
+        <v>3496</v>
       </c>
       <c r="C652" s="4" t="s">
-        <v>3495</v>
-      </c>
-      <c r="D652" s="11" t="s">
         <v>3496</v>
       </c>
-      <c r="E652" s="26" t="s">
-        <v>2110</v>
+      <c r="D652" s="4" t="s">
+        <v>3496</v>
+      </c>
+      <c r="E652" s="27" t="n">
+        <v>45528</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>